<commit_message>
feat(ADMIN_TECHNIQUE): [statistiques] fonction export - users #885
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="Stats Globales" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Liste Structures" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Liste utilisateurs" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t xml:space="preserve">Date et heure</t>
   </si>
@@ -147,6 +148,34 @@
   </si>
   <si>
     <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur
+ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur
+Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur
+Prénom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur
+Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur
+Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure
+ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure
+Nom</t>
   </si>
 </sst>
 </file>
@@ -252,7 +281,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -297,6 +326,18 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -317,7 +358,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -545,7 +586,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1804,4 +1845,67 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="11" width="25.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="61.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="25.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="67.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="8" style="11" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1021" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="13" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(ADMIN_TECHNIQUE): [statistiques] fonction export - users #885 (#937)
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="Stats Globales" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Liste Structures" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Liste utilisateurs" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t xml:space="preserve">Date et heure</t>
   </si>
@@ -147,6 +148,34 @@
   </si>
   <si>
     <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur
+ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur
+Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur
+Prénom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur
+Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur
+Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure
+ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure
+Nom</t>
   </si>
 </sst>
 </file>
@@ -252,7 +281,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -297,6 +326,18 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -317,7 +358,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -545,7 +586,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1804,4 +1845,67 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="11" width="25.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="61.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="25.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="67.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="8" style="11" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1021" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="13" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(export): add non-verified users
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Stats Globales" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t xml:space="preserve">Date et heure</t>
   </si>
@@ -168,6 +168,10 @@
   <si>
     <t xml:space="preserve">Utilisateur
 Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur
+Vérifié</t>
   </si>
   <si>
     <t xml:space="preserve">Structure
@@ -361,7 +365,7 @@
   </sheetPr>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1856,10 +1860,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1868,11 +1872,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="12" width="25.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="61.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="12" width="25.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="12" width="12.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="12" width="67.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="8" style="12" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1021" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="12" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="12" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="12" width="67.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="9" style="12" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1022" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1897,7 +1902,9 @@
       <c r="G1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AMG1" s="0"/>
+      <c r="H1" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>

</xml_diff>

<commit_message>
bug(export): problèmes export domifa #1034 (#1035)
* bug(export): problèmes export domifa #1034

* bug(export): problèmes export domifa #1034

* fix: colonne manquante

Co-authored-by: Yassine R <riffi.yassine@gmail.com>
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VBOXSVR\_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/www/beta/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405AFF38-32B2-E14E-BC4B-581D30A95A03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23220" windowHeight="17500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats Globales" sheetId="1" r:id="rId1"/>
     <sheet name="Liste Structures" sheetId="2" r:id="rId2"/>
     <sheet name="Liste utilisateurs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Date et heure</t>
   </si>
@@ -180,12 +181,15 @@
   <si>
     <t>Structure
 Nom</t>
+  </si>
+  <si>
+    <t>Vérifié</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy&quot; à &quot;hh:mm"/>
   </numFmts>
@@ -242,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
@@ -263,12 +267,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -283,6 +281,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,215 +570,215 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="7" customWidth="1"/>
-    <col min="5" max="1025" width="14.42578125" style="7" customWidth="1"/>
-    <col min="1026" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="26.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" style="7" customWidth="1"/>
+    <col min="5" max="1025" width="14.5" style="7" customWidth="1"/>
+    <col min="1026" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="B1" s="10"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="B4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="B5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="B6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="B7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="B8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+      <c r="B9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="B10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="B13" s="9"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+      <c r="B14" s="9"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="B15" s="9"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
+      <c r="B16" s="9"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="B18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="14"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+      <c r="B19" s="12"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="11"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+      <c r="B23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="11"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="11"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="11"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+      <c r="B26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="14"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="11"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
+      <c r="B28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="11"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
+      <c r="B29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="11"/>
+      <c r="B30" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -780,35 +787,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK183"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="41.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="3" customWidth="1"/>
     <col min="9" max="10" width="13" style="5" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="6.1640625" style="5" customWidth="1"/>
     <col min="12" max="12" width="33" style="3" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" style="5" customWidth="1"/>
     <col min="14" max="14" width="35" style="3" customWidth="1"/>
-    <col min="15" max="15" width="44.28515625" style="3" customWidth="1"/>
-    <col min="16" max="1025" width="8.7109375" style="3" customWidth="1"/>
-    <col min="1026" max="16384" width="9.140625" style="7"/>
+    <col min="15" max="15" width="44.33203125" style="3" customWidth="1"/>
+    <col min="16" max="1025" width="8.6640625" style="3" customWidth="1"/>
+    <col min="1026" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -855,7 +862,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D2" s="4"/>
       <c r="F2" s="4"/>
       <c r="I2" s="4"/>
@@ -863,150 +870,150 @@
       <c r="K2" s="4"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
       <c r="I24" s="4"/>
@@ -1014,10 +1021,10 @@
       <c r="K24" s="4"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D26" s="4"/>
       <c r="F26" s="4"/>
       <c r="I26" s="4"/>
@@ -1025,21 +1032,21 @@
       <c r="K26" s="4"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
       <c r="I29" s="4"/>
@@ -1047,79 +1054,79 @@
       <c r="K29" s="4"/>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="6"/>
     </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="6"/>
     </row>
-    <row r="38" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="6"/>
     </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="6"/>
     </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D42" s="4"/>
       <c r="F42" s="4"/>
       <c r="I42" s="4"/>
@@ -1127,7 +1134,7 @@
       <c r="K42" s="4"/>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
       <c r="I43" s="4"/>
@@ -1135,7 +1142,7 @@
       <c r="K43" s="4"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D44" s="4"/>
       <c r="F44" s="4"/>
       <c r="I44" s="4"/>
@@ -1143,43 +1150,43 @@
       <c r="K44" s="4"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="6"/>
     </row>
-    <row r="50" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D52" s="4"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="6"/>
     </row>
-    <row r="53" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D53" s="4"/>
       <c r="F53" s="4"/>
       <c r="I53" s="4"/>
@@ -1187,16 +1194,16 @@
       <c r="K53" s="4"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D57" s="4"/>
       <c r="F57" s="4"/>
       <c r="I57" s="4"/>
@@ -1204,7 +1211,7 @@
       <c r="K57" s="4"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D58" s="4"/>
       <c r="F58" s="4"/>
       <c r="I58" s="4"/>
@@ -1212,10 +1219,10 @@
       <c r="K58" s="4"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D60" s="4"/>
       <c r="F60" s="4"/>
       <c r="I60" s="4"/>
@@ -1223,34 +1230,34 @@
       <c r="K60" s="4"/>
       <c r="L60" s="6"/>
     </row>
-    <row r="61" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D62" s="4"/>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D64" s="4"/>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D66" s="4"/>
       <c r="F66" s="4"/>
       <c r="I66" s="4"/>
@@ -1258,42 +1265,42 @@
       <c r="K66" s="4"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D67" s="4"/>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D68" s="4"/>
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D69" s="4"/>
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D70" s="4"/>
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D71" s="4"/>
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
       <c r="L71" s="6"/>
     </row>
-    <row r="72" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D72" s="4"/>
       <c r="F72" s="4"/>
       <c r="I72" s="4"/>
@@ -1301,17 +1308,17 @@
       <c r="K72" s="4"/>
       <c r="L72" s="6"/>
     </row>
-    <row r="73" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D74" s="4"/>
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
       <c r="L74" s="6"/>
     </row>
-    <row r="75" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D75" s="4"/>
       <c r="F75" s="4"/>
       <c r="I75" s="4"/>
@@ -1319,10 +1326,10 @@
       <c r="K75" s="4"/>
       <c r="L75" s="6"/>
     </row>
-    <row r="76" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D77" s="4"/>
       <c r="F77" s="4"/>
       <c r="I77" s="4"/>
@@ -1330,20 +1337,20 @@
       <c r="K77" s="4"/>
       <c r="L77" s="6"/>
     </row>
-    <row r="78" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D79" s="4"/>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
       <c r="L79" s="6"/>
     </row>
-    <row r="80" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D80" s="4"/>
     </row>
-    <row r="81" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D81" s="4"/>
       <c r="F81" s="4"/>
       <c r="I81" s="4"/>
@@ -1351,24 +1358,24 @@
       <c r="K81" s="4"/>
       <c r="L81" s="6"/>
     </row>
-    <row r="82" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D82" s="4"/>
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D84" s="4"/>
       <c r="I84" s="4"/>
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
       <c r="L84" s="6"/>
     </row>
-    <row r="85" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D85" s="4"/>
       <c r="F85" s="4"/>
       <c r="I85" s="4"/>
@@ -1376,17 +1383,17 @@
       <c r="K85" s="4"/>
       <c r="L85" s="6"/>
     </row>
-    <row r="86" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D86" s="4"/>
       <c r="I86" s="4"/>
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
       <c r="L86" s="6"/>
     </row>
-    <row r="87" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D88" s="4"/>
       <c r="F88" s="4"/>
       <c r="I88" s="4"/>
@@ -1394,14 +1401,14 @@
       <c r="K88" s="4"/>
       <c r="L88" s="6"/>
     </row>
-    <row r="89" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D89" s="4"/>
       <c r="I89" s="4"/>
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
       <c r="L89" s="6"/>
     </row>
-    <row r="90" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D90" s="4"/>
       <c r="F90" s="4"/>
       <c r="I90" s="4"/>
@@ -1409,7 +1416,7 @@
       <c r="K90" s="4"/>
       <c r="L90" s="6"/>
     </row>
-    <row r="91" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D91" s="4"/>
       <c r="F91" s="4"/>
       <c r="I91" s="4"/>
@@ -1417,7 +1424,7 @@
       <c r="K91" s="4"/>
       <c r="L91" s="6"/>
     </row>
-    <row r="92" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D92" s="4"/>
       <c r="F92" s="4"/>
       <c r="I92" s="4"/>
@@ -1425,7 +1432,7 @@
       <c r="K92" s="4"/>
       <c r="L92" s="6"/>
     </row>
-    <row r="93" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D93" s="4"/>
       <c r="F93" s="4"/>
       <c r="I93" s="4"/>
@@ -1433,28 +1440,28 @@
       <c r="K93" s="4"/>
       <c r="L93" s="6"/>
     </row>
-    <row r="94" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D94" s="4"/>
       <c r="I94" s="4"/>
       <c r="J94" s="4"/>
       <c r="K94" s="4"/>
       <c r="L94" s="6"/>
     </row>
-    <row r="95" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D95" s="4"/>
       <c r="I95" s="4"/>
       <c r="J95" s="4"/>
       <c r="K95" s="4"/>
       <c r="L95" s="6"/>
     </row>
-    <row r="96" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D96" s="4"/>
       <c r="I96" s="4"/>
       <c r="J96" s="4"/>
       <c r="K96" s="4"/>
       <c r="L96" s="6"/>
     </row>
-    <row r="97" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D97" s="4"/>
       <c r="F97" s="4"/>
       <c r="I97" s="4"/>
@@ -1462,14 +1469,14 @@
       <c r="K97" s="4"/>
       <c r="L97" s="6"/>
     </row>
-    <row r="98" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D98" s="4"/>
       <c r="I98" s="4"/>
       <c r="J98" s="4"/>
       <c r="K98" s="4"/>
       <c r="L98" s="6"/>
     </row>
-    <row r="99" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D99" s="4"/>
       <c r="F99" s="4"/>
       <c r="I99" s="4"/>
@@ -1477,7 +1484,7 @@
       <c r="K99" s="4"/>
       <c r="L99" s="6"/>
     </row>
-    <row r="100" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D100" s="4"/>
       <c r="F100" s="4"/>
       <c r="I100" s="4"/>
@@ -1485,7 +1492,7 @@
       <c r="K100" s="4"/>
       <c r="L100" s="6"/>
     </row>
-    <row r="101" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D101" s="4"/>
       <c r="F101" s="4"/>
       <c r="I101" s="4"/>
@@ -1493,7 +1500,7 @@
       <c r="K101" s="4"/>
       <c r="L101" s="6"/>
     </row>
-    <row r="102" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D102" s="4"/>
       <c r="F102" s="4"/>
       <c r="I102" s="4"/>
@@ -1501,21 +1508,21 @@
       <c r="K102" s="4"/>
       <c r="L102" s="6"/>
     </row>
-    <row r="103" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D103" s="4"/>
       <c r="I103" s="4"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
       <c r="L103" s="6"/>
     </row>
-    <row r="104" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D104" s="4"/>
       <c r="I104" s="4"/>
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
       <c r="L104" s="6"/>
     </row>
-    <row r="105" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D105" s="4"/>
       <c r="F105" s="4"/>
       <c r="I105" s="4"/>
@@ -1523,7 +1530,7 @@
       <c r="K105" s="4"/>
       <c r="L105" s="6"/>
     </row>
-    <row r="106" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D106" s="4"/>
       <c r="F106" s="4"/>
       <c r="I106" s="4"/>
@@ -1531,14 +1538,14 @@
       <c r="K106" s="4"/>
       <c r="L106" s="6"/>
     </row>
-    <row r="107" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D107" s="4"/>
       <c r="I107" s="4"/>
       <c r="J107" s="4"/>
       <c r="K107" s="4"/>
       <c r="L107" s="6"/>
     </row>
-    <row r="108" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D108" s="4"/>
       <c r="F108" s="4"/>
       <c r="I108" s="4"/>
@@ -1546,7 +1553,7 @@
       <c r="K108" s="4"/>
       <c r="L108" s="6"/>
     </row>
-    <row r="109" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D109" s="4"/>
       <c r="F109" s="4"/>
       <c r="I109" s="4"/>
@@ -1554,14 +1561,14 @@
       <c r="K109" s="4"/>
       <c r="L109" s="6"/>
     </row>
-    <row r="110" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D110" s="4"/>
       <c r="I110" s="4"/>
       <c r="J110" s="4"/>
       <c r="K110" s="4"/>
       <c r="L110" s="6"/>
     </row>
-    <row r="111" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D111" s="4"/>
       <c r="F111" s="4"/>
       <c r="I111" s="4"/>
@@ -1569,28 +1576,28 @@
       <c r="K111" s="4"/>
       <c r="L111" s="6"/>
     </row>
-    <row r="112" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D112" s="4"/>
       <c r="I112" s="4"/>
       <c r="J112" s="4"/>
       <c r="K112" s="4"/>
       <c r="L112" s="6"/>
     </row>
-    <row r="113" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D113" s="4"/>
       <c r="I113" s="4"/>
       <c r="J113" s="4"/>
       <c r="K113" s="4"/>
       <c r="L113" s="6"/>
     </row>
-    <row r="114" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D114" s="4"/>
       <c r="I114" s="4"/>
       <c r="J114" s="4"/>
       <c r="K114" s="4"/>
       <c r="L114" s="6"/>
     </row>
-    <row r="115" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D115" s="4"/>
       <c r="F115" s="4"/>
       <c r="I115" s="4"/>
@@ -1598,7 +1605,7 @@
       <c r="K115" s="4"/>
       <c r="L115" s="6"/>
     </row>
-    <row r="116" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D116" s="4"/>
       <c r="F116" s="4"/>
       <c r="I116" s="4"/>
@@ -1606,7 +1613,7 @@
       <c r="K116" s="4"/>
       <c r="L116" s="6"/>
     </row>
-    <row r="117" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D117" s="4"/>
       <c r="F117" s="4"/>
       <c r="I117" s="4"/>
@@ -1614,7 +1621,7 @@
       <c r="K117" s="4"/>
       <c r="L117" s="6"/>
     </row>
-    <row r="118" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D118" s="4"/>
       <c r="F118" s="4"/>
       <c r="I118" s="4"/>
@@ -1622,7 +1629,7 @@
       <c r="K118" s="4"/>
       <c r="L118" s="6"/>
     </row>
-    <row r="119" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D119" s="4"/>
       <c r="F119" s="4"/>
       <c r="I119" s="4"/>
@@ -1630,7 +1637,7 @@
       <c r="K119" s="4"/>
       <c r="L119" s="6"/>
     </row>
-    <row r="120" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D120" s="4"/>
       <c r="F120" s="4"/>
       <c r="I120" s="4"/>
@@ -1638,42 +1645,42 @@
       <c r="K120" s="4"/>
       <c r="L120" s="6"/>
     </row>
-    <row r="121" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D121" s="4"/>
       <c r="I121" s="4"/>
       <c r="J121" s="4"/>
       <c r="K121" s="4"/>
       <c r="L121" s="6"/>
     </row>
-    <row r="122" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D122" s="4"/>
       <c r="I122" s="4"/>
       <c r="J122" s="4"/>
       <c r="K122" s="4"/>
       <c r="L122" s="6"/>
     </row>
-    <row r="123" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D123" s="4"/>
       <c r="I123" s="4"/>
       <c r="J123" s="4"/>
       <c r="K123" s="4"/>
       <c r="L123" s="6"/>
     </row>
-    <row r="124" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D124" s="4"/>
       <c r="I124" s="4"/>
       <c r="J124" s="4"/>
       <c r="K124" s="4"/>
       <c r="L124" s="6"/>
     </row>
-    <row r="125" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D125" s="4"/>
       <c r="I125" s="4"/>
       <c r="J125" s="4"/>
       <c r="K125" s="4"/>
       <c r="L125" s="6"/>
     </row>
-    <row r="126" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D126" s="4"/>
       <c r="F126" s="4"/>
       <c r="I126" s="4"/>
@@ -1681,34 +1688,34 @@
       <c r="K126" s="4"/>
       <c r="L126" s="6"/>
     </row>
-    <row r="127" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D127" s="4"/>
       <c r="I127" s="4"/>
       <c r="J127" s="4"/>
       <c r="K127" s="4"/>
       <c r="L127" s="6"/>
     </row>
-    <row r="128" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D128" s="4"/>
       <c r="I128" s="4"/>
       <c r="J128" s="4"/>
       <c r="K128" s="4"/>
       <c r="L128" s="6"/>
     </row>
-    <row r="129" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D130" s="4"/>
       <c r="I130" s="4"/>
       <c r="J130" s="4"/>
       <c r="K130" s="4"/>
       <c r="L130" s="6"/>
     </row>
-    <row r="131" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D132" s="4"/>
       <c r="F132" s="4"/>
       <c r="I132" s="4"/>
@@ -1716,103 +1723,103 @@
       <c r="K132" s="4"/>
       <c r="L132" s="6"/>
     </row>
-    <row r="133" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D133" s="4"/>
       <c r="I133" s="4"/>
       <c r="J133" s="4"/>
       <c r="K133" s="4"/>
       <c r="L133" s="6"/>
     </row>
-    <row r="134" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D134" s="4"/>
       <c r="I134" s="4"/>
       <c r="J134" s="4"/>
       <c r="K134" s="4"/>
       <c r="L134" s="6"/>
     </row>
-    <row r="135" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D135" s="4"/>
       <c r="I135" s="4"/>
       <c r="J135" s="4"/>
       <c r="K135" s="4"/>
       <c r="L135" s="6"/>
     </row>
-    <row r="136" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D136" s="4"/>
       <c r="I136" s="4"/>
       <c r="J136" s="4"/>
       <c r="K136" s="4"/>
       <c r="L136" s="6"/>
     </row>
-    <row r="137" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D139" s="4"/>
       <c r="I139" s="4"/>
       <c r="J139" s="4"/>
       <c r="K139" s="4"/>
       <c r="L139" s="6"/>
     </row>
-    <row r="140" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D140" s="4"/>
       <c r="I140" s="4"/>
       <c r="J140" s="4"/>
       <c r="K140" s="4"/>
       <c r="L140" s="6"/>
     </row>
-    <row r="141" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="141" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D141" s="4"/>
       <c r="I141" s="4"/>
       <c r="J141" s="4"/>
       <c r="K141" s="4"/>
       <c r="L141" s="6"/>
     </row>
-    <row r="142" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="142" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D142" s="4"/>
       <c r="I142" s="4"/>
       <c r="J142" s="4"/>
       <c r="K142" s="4"/>
       <c r="L142" s="6"/>
     </row>
-    <row r="143" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D143" s="4"/>
       <c r="I143" s="4"/>
       <c r="J143" s="4"/>
       <c r="K143" s="4"/>
       <c r="L143" s="6"/>
     </row>
-    <row r="144" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D145" s="4"/>
       <c r="I145" s="4"/>
       <c r="J145" s="4"/>
       <c r="K145" s="4"/>
       <c r="L145" s="6"/>
     </row>
-    <row r="146" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D146" s="4"/>
       <c r="I146" s="4"/>
       <c r="J146" s="4"/>
       <c r="K146" s="4"/>
       <c r="L146" s="6"/>
     </row>
-    <row r="147" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D147" s="4"/>
       <c r="I147" s="4"/>
       <c r="J147" s="4"/>
       <c r="K147" s="4"/>
       <c r="L147" s="6"/>
     </row>
-    <row r="148" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D148" s="4"/>
     </row>
-    <row r="149" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D149" s="4"/>
       <c r="F149" s="4"/>
       <c r="I149" s="4"/>
@@ -1820,49 +1827,49 @@
       <c r="K149" s="4"/>
       <c r="L149" s="6"/>
     </row>
-    <row r="150" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D150" s="4"/>
       <c r="I150" s="4"/>
       <c r="J150" s="4"/>
       <c r="K150" s="4"/>
       <c r="L150" s="6"/>
     </row>
-    <row r="151" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D151" s="4"/>
       <c r="I151" s="4"/>
       <c r="J151" s="4"/>
       <c r="K151" s="4"/>
       <c r="L151" s="6"/>
     </row>
-    <row r="152" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D152" s="4"/>
       <c r="I152" s="4"/>
       <c r="J152" s="4"/>
       <c r="K152" s="4"/>
       <c r="L152" s="6"/>
     </row>
-    <row r="153" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D153" s="4"/>
       <c r="I153" s="4"/>
       <c r="J153" s="4"/>
       <c r="K153" s="4"/>
       <c r="L153" s="6"/>
     </row>
-    <row r="154" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D154" s="4"/>
       <c r="I154" s="4"/>
       <c r="J154" s="4"/>
       <c r="K154" s="4"/>
       <c r="L154" s="6"/>
     </row>
-    <row r="155" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D155" s="4"/>
       <c r="I155" s="4"/>
       <c r="J155" s="4"/>
       <c r="K155" s="4"/>
       <c r="L155" s="6"/>
     </row>
-    <row r="156" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D156" s="4"/>
       <c r="F156" s="4"/>
       <c r="I156" s="4"/>
@@ -1870,7 +1877,7 @@
       <c r="K156" s="4"/>
       <c r="L156" s="6"/>
     </row>
-    <row r="157" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D157" s="4"/>
       <c r="F157" s="4"/>
       <c r="I157" s="4"/>
@@ -1878,21 +1885,21 @@
       <c r="K157" s="4"/>
       <c r="L157" s="6"/>
     </row>
-    <row r="158" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D158" s="4"/>
       <c r="I158" s="4"/>
       <c r="J158" s="4"/>
       <c r="K158" s="4"/>
       <c r="L158" s="6"/>
     </row>
-    <row r="159" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D159" s="4"/>
       <c r="I159" s="4"/>
       <c r="J159" s="4"/>
       <c r="K159" s="4"/>
       <c r="L159" s="6"/>
     </row>
-    <row r="160" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D160" s="4"/>
       <c r="F160" s="4"/>
       <c r="I160" s="4"/>
@@ -1900,7 +1907,7 @@
       <c r="K160" s="4"/>
       <c r="L160" s="6"/>
     </row>
-    <row r="161" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="161" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D161" s="4"/>
       <c r="F161" s="4"/>
       <c r="I161" s="4"/>
@@ -1908,21 +1915,21 @@
       <c r="K161" s="4"/>
       <c r="L161" s="6"/>
     </row>
-    <row r="162" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="162" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D162" s="4"/>
       <c r="I162" s="4"/>
       <c r="J162" s="4"/>
       <c r="K162" s="4"/>
       <c r="L162" s="6"/>
     </row>
-    <row r="163" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="163" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D163" s="4"/>
       <c r="I163" s="4"/>
       <c r="J163" s="4"/>
       <c r="K163" s="4"/>
       <c r="L163" s="6"/>
     </row>
-    <row r="164" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="164" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D164" s="4"/>
       <c r="F164" s="4"/>
       <c r="I164" s="4"/>
@@ -1930,84 +1937,84 @@
       <c r="K164" s="4"/>
       <c r="L164" s="6"/>
     </row>
-    <row r="165" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="165" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D165" s="4"/>
       <c r="I165" s="4"/>
       <c r="J165" s="4"/>
       <c r="K165" s="4"/>
       <c r="L165" s="6"/>
     </row>
-    <row r="166" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="166" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D166" s="4"/>
       <c r="I166" s="4"/>
       <c r="J166" s="4"/>
       <c r="K166" s="4"/>
       <c r="L166" s="6"/>
     </row>
-    <row r="167" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="167" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D167" s="4"/>
       <c r="I167" s="4"/>
       <c r="J167" s="4"/>
       <c r="K167" s="4"/>
       <c r="L167" s="6"/>
     </row>
-    <row r="168" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="168" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D168" s="4"/>
       <c r="I168" s="4"/>
       <c r="J168" s="4"/>
       <c r="K168" s="4"/>
       <c r="L168" s="6"/>
     </row>
-    <row r="169" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="169" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D169" s="4"/>
       <c r="I169" s="4"/>
       <c r="J169" s="4"/>
       <c r="K169" s="4"/>
       <c r="L169" s="6"/>
     </row>
-    <row r="170" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="170" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D170" s="4"/>
       <c r="I170" s="4"/>
       <c r="J170" s="4"/>
       <c r="K170" s="4"/>
       <c r="L170" s="6"/>
     </row>
-    <row r="171" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="171" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D171" s="4"/>
       <c r="I171" s="4"/>
       <c r="J171" s="4"/>
       <c r="K171" s="4"/>
       <c r="L171" s="6"/>
     </row>
-    <row r="172" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="172" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D172" s="4"/>
       <c r="I172" s="4"/>
       <c r="J172" s="4"/>
       <c r="K172" s="4"/>
       <c r="L172" s="6"/>
     </row>
-    <row r="173" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="173" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D173" s="4"/>
       <c r="I173" s="4"/>
       <c r="J173" s="4"/>
       <c r="K173" s="4"/>
       <c r="L173" s="6"/>
     </row>
-    <row r="174" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="174" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D174" s="4"/>
       <c r="I174" s="4"/>
       <c r="J174" s="4"/>
       <c r="K174" s="4"/>
       <c r="L174" s="6"/>
     </row>
-    <row r="175" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="175" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D175" s="4"/>
       <c r="I175" s="4"/>
       <c r="J175" s="4"/>
       <c r="K175" s="4"/>
       <c r="L175" s="6"/>
     </row>
-    <row r="176" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="176" spans="4:12" x14ac:dyDescent="0.15">
       <c r="D176" s="4"/>
       <c r="F176" s="4"/>
       <c r="I176" s="4"/>
@@ -2015,25 +2022,25 @@
       <c r="K176" s="4"/>
       <c r="L176" s="6"/>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D177" s="4"/>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D178" s="4"/>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D179" s="4"/>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D180" s="4"/>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D181" s="4"/>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D182" s="4"/>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D183" s="4"/>
     </row>
   </sheetData>
@@ -2043,53 +2050,56 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="10" customWidth="1"/>
-    <col min="2" max="3" width="25.5703125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="62" style="10" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="67.140625" style="10" customWidth="1"/>
-    <col min="8" max="1020" width="11.5703125" style="10"/>
-    <col min="1021" max="1022" width="8.7109375" style="7" customWidth="1"/>
-    <col min="1023" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="12.83203125" style="8" customWidth="1"/>
+    <col min="2" max="3" width="25.5" style="8" customWidth="1"/>
+    <col min="4" max="4" width="62" style="8" customWidth="1"/>
+    <col min="5" max="5" width="25.5" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
+    <col min="7" max="7" width="67.1640625" style="8" customWidth="1"/>
+    <col min="8" max="1020" width="11.5" style="8"/>
+    <col min="1021" max="1022" width="8.6640625" style="7" customWidth="1"/>
+    <col min="1023" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:1024" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AMG1" s="7"/>
-      <c r="AMH1" s="7"/>
-      <c r="AMI1" s="7"/>
-      <c r="AMJ1" s="7"/>
+      <c r="H1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AMG1" s="15"/>
+      <c r="AMH1" s="15"/>
+      <c r="AMI1" s="15"/>
+      <c r="AMJ1" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
feat(STATS_DOMIFA): renommage et ajout colonne dans page + export #1295
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/www/beta/domifa/packages/backend/src/excel/_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VBOXSVR\_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405AFF38-32B2-E14E-BC4B-581D30A95A03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23220" windowHeight="17500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="23220" windowHeight="17505" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stats Globales" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Date et heure</t>
   </si>
@@ -129,9 +128,6 @@
   </si>
   <si>
     <t>Comptes</t>
-  </si>
-  <si>
-    <t>Domiciliés</t>
   </si>
   <si>
     <t>Dernière connexion</t>
@@ -189,7 +185,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy&quot; à &quot;hh:mm"/>
   </numFmts>
@@ -570,30 +566,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="7" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" style="7" customWidth="1"/>
-    <col min="5" max="1025" width="14.5" style="7" customWidth="1"/>
-    <col min="1026" max="16384" width="9.1640625" style="7"/>
+    <col min="1" max="1" width="26.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="7" customWidth="1"/>
+    <col min="5" max="1025" width="14.42578125" style="7" customWidth="1"/>
+    <col min="1026" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -604,7 +600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -612,7 +608,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -620,7 +616,7 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
@@ -628,7 +624,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
@@ -636,7 +632,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>8</v>
       </c>
@@ -644,7 +640,7 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
@@ -652,7 +648,7 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
@@ -660,18 +656,18 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
@@ -679,7 +675,7 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>12</v>
       </c>
@@ -687,7 +683,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
@@ -695,7 +691,7 @@
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>14</v>
       </c>
@@ -703,11 +699,11 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>15</v>
       </c>
@@ -715,66 +711,66 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="12"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="9"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="9"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="9"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="9"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="9"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="12"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="9"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="9"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>26</v>
       </c>
@@ -787,35 +783,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK183"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AML183"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="41.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="3" customWidth="1"/>
-    <col min="9" max="10" width="13" style="5" customWidth="1"/>
-    <col min="11" max="11" width="6.1640625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="33" style="3" customWidth="1"/>
-    <col min="13" max="13" width="7.83203125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="35" style="3" customWidth="1"/>
-    <col min="15" max="15" width="44.33203125" style="3" customWidth="1"/>
-    <col min="16" max="1025" width="8.6640625" style="3" customWidth="1"/>
-    <col min="1026" max="16384" width="9.1640625" style="7"/>
+    <col min="1" max="1" width="5.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="3" customWidth="1"/>
+    <col min="8" max="9" width="12.42578125" style="3" customWidth="1"/>
+    <col min="10" max="11" width="13" style="5" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="33" style="3" customWidth="1"/>
+    <col min="14" max="14" width="7.85546875" style="5" customWidth="1"/>
+    <col min="15" max="15" width="35" style="3" customWidth="1"/>
+    <col min="16" max="16" width="44.28515625" style="3" customWidth="1"/>
+    <col min="17" max="1026" width="8.7109375" style="3" customWidth="1"/>
+    <col min="1027" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -838,1209 +834,1212 @@
         <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L2" s="4"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" s="4"/>
-      <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L3" s="4"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D4" s="4"/>
-      <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L4" s="4"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D5" s="4"/>
-      <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L5" s="4"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D6" s="4"/>
-      <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L6" s="4"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D7" s="4"/>
-      <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L7" s="4"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D8" s="4"/>
-      <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L8" s="4"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D9" s="4"/>
-      <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L9" s="4"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D10" s="4"/>
-      <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L10" s="4"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D11" s="4"/>
-      <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L11" s="4"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D12" s="4"/>
-      <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L12" s="4"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D13" s="4"/>
-      <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L13" s="4"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D14" s="4"/>
-      <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L14" s="4"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D15" s="4"/>
-      <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="L15" s="4"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D17" s="4"/>
-      <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L17" s="4"/>
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D18" s="4"/>
-      <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L18" s="4"/>
+      <c r="M18" s="6"/>
+    </row>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D19" s="4"/>
-      <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L19" s="4"/>
+      <c r="M19" s="6"/>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D20" s="4"/>
-      <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L20" s="4"/>
+      <c r="M20" s="6"/>
+    </row>
+    <row r="21" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D21" s="4"/>
-      <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="6"/>
-    </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L21" s="4"/>
+      <c r="M21" s="6"/>
+    </row>
+    <row r="22" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D22" s="4"/>
-      <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="6"/>
-    </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L22" s="4"/>
+      <c r="M22" s="6"/>
+    </row>
+    <row r="23" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D23" s="4"/>
-      <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L23" s="4"/>
+      <c r="M23" s="6"/>
+    </row>
+    <row r="24" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="6"/>
-    </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L24" s="4"/>
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="26" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="6"/>
-    </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L26" s="4"/>
+      <c r="M26" s="6"/>
+    </row>
+    <row r="27" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D27" s="4"/>
-      <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="6"/>
-    </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L27" s="4"/>
+      <c r="M27" s="6"/>
+    </row>
+    <row r="28" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D28" s="4"/>
-      <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="6"/>
-    </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L28" s="4"/>
+      <c r="M28" s="6"/>
+    </row>
+    <row r="29" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L29" s="4"/>
+      <c r="M29" s="6"/>
+    </row>
+    <row r="30" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D30" s="4"/>
-      <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="6"/>
-    </row>
-    <row r="31" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L30" s="4"/>
+      <c r="M30" s="6"/>
+    </row>
+    <row r="31" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D31" s="4"/>
-      <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="6"/>
-    </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L31" s="4"/>
+      <c r="M31" s="6"/>
+    </row>
+    <row r="32" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D32" s="4"/>
-      <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="6"/>
-    </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L32" s="4"/>
+      <c r="M32" s="6"/>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D33" s="4"/>
-      <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="6"/>
-    </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L33" s="4"/>
+      <c r="M33" s="6"/>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D34" s="4"/>
-      <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
-      <c r="L34" s="6"/>
-    </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L34" s="4"/>
+      <c r="M34" s="6"/>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="36" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="37" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D37" s="4"/>
-      <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="6"/>
-    </row>
-    <row r="38" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L37" s="4"/>
+      <c r="M37" s="6"/>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="39" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D39" s="4"/>
-      <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="6"/>
-    </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L39" s="4"/>
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D40" s="4"/>
-      <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="6"/>
-    </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L40" s="4"/>
+      <c r="M40" s="6"/>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D41" s="4"/>
-      <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="6"/>
-    </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L41" s="4"/>
+      <c r="M41" s="6"/>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="6"/>
-    </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L42" s="4"/>
+      <c r="M42" s="6"/>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="6"/>
-    </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L43" s="4"/>
+      <c r="M43" s="6"/>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="6"/>
-    </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L44" s="4"/>
+      <c r="M44" s="6"/>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D45" s="4"/>
-      <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
-      <c r="L45" s="6"/>
-    </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L45" s="4"/>
+      <c r="M45" s="6"/>
+    </row>
+    <row r="46" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="47" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="48" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="49" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D49" s="4"/>
-      <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
-      <c r="L49" s="6"/>
-    </row>
-    <row r="50" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L49" s="4"/>
+      <c r="M49" s="6"/>
+    </row>
+    <row r="50" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="51" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="52" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D52" s="4"/>
-      <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
-      <c r="L52" s="6"/>
-    </row>
-    <row r="53" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L52" s="4"/>
+      <c r="M52" s="6"/>
+    </row>
+    <row r="53" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D53" s="4"/>
       <c r="F53" s="4"/>
-      <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
-      <c r="L53" s="6"/>
-    </row>
-    <row r="54" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L53" s="4"/>
+      <c r="M53" s="6"/>
+    </row>
+    <row r="54" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="55" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="56" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="57" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
-      <c r="L57" s="6"/>
-    </row>
-    <row r="58" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L57" s="4"/>
+      <c r="M57" s="6"/>
+    </row>
+    <row r="58" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
-      <c r="L58" s="6"/>
-    </row>
-    <row r="59" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L58" s="4"/>
+      <c r="M58" s="6"/>
+    </row>
+    <row r="59" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="60" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D60" s="4"/>
       <c r="F60" s="4"/>
-      <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
-      <c r="L60" s="6"/>
-    </row>
-    <row r="61" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L60" s="4"/>
+      <c r="M60" s="6"/>
+    </row>
+    <row r="61" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D61" s="4"/>
-      <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
-      <c r="L61" s="6"/>
-    </row>
-    <row r="62" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L61" s="4"/>
+      <c r="M61" s="6"/>
+    </row>
+    <row r="62" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D62" s="4"/>
-      <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
-      <c r="L62" s="6"/>
-    </row>
-    <row r="63" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L62" s="4"/>
+      <c r="M62" s="6"/>
+    </row>
+    <row r="63" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="64" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D64" s="4"/>
-      <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
-      <c r="L64" s="6"/>
-    </row>
-    <row r="65" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L64" s="4"/>
+      <c r="M64" s="6"/>
+    </row>
+    <row r="65" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="66" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D66" s="4"/>
       <c r="F66" s="4"/>
-      <c r="I66" s="4"/>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
-      <c r="L66" s="6"/>
-    </row>
-    <row r="67" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L66" s="4"/>
+      <c r="M66" s="6"/>
+    </row>
+    <row r="67" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D67" s="4"/>
-      <c r="I67" s="4"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
-      <c r="L67" s="6"/>
-    </row>
-    <row r="68" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L67" s="4"/>
+      <c r="M67" s="6"/>
+    </row>
+    <row r="68" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D68" s="4"/>
-      <c r="I68" s="4"/>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
-      <c r="L68" s="6"/>
-    </row>
-    <row r="69" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L68" s="4"/>
+      <c r="M68" s="6"/>
+    </row>
+    <row r="69" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D69" s="4"/>
-      <c r="I69" s="4"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
-      <c r="L69" s="6"/>
-    </row>
-    <row r="70" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L69" s="4"/>
+      <c r="M69" s="6"/>
+    </row>
+    <row r="70" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D70" s="4"/>
-      <c r="I70" s="4"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
-      <c r="L70" s="6"/>
-    </row>
-    <row r="71" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L70" s="4"/>
+      <c r="M70" s="6"/>
+    </row>
+    <row r="71" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D71" s="4"/>
-      <c r="I71" s="4"/>
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
-      <c r="L71" s="6"/>
-    </row>
-    <row r="72" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L71" s="4"/>
+      <c r="M71" s="6"/>
+    </row>
+    <row r="72" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D72" s="4"/>
       <c r="F72" s="4"/>
-      <c r="I72" s="4"/>
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
-      <c r="L72" s="6"/>
-    </row>
-    <row r="73" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L72" s="4"/>
+      <c r="M72" s="6"/>
+    </row>
+    <row r="73" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="74" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D74" s="4"/>
-      <c r="I74" s="4"/>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
-      <c r="L74" s="6"/>
-    </row>
-    <row r="75" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L74" s="4"/>
+      <c r="M74" s="6"/>
+    </row>
+    <row r="75" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D75" s="4"/>
       <c r="F75" s="4"/>
-      <c r="I75" s="4"/>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
-      <c r="L75" s="6"/>
-    </row>
-    <row r="76" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L75" s="4"/>
+      <c r="M75" s="6"/>
+    </row>
+    <row r="76" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="77" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D77" s="4"/>
       <c r="F77" s="4"/>
-      <c r="I77" s="4"/>
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
-      <c r="L77" s="6"/>
-    </row>
-    <row r="78" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L77" s="4"/>
+      <c r="M77" s="6"/>
+    </row>
+    <row r="78" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="79" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D79" s="4"/>
-      <c r="I79" s="4"/>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
-      <c r="L79" s="6"/>
-    </row>
-    <row r="80" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L79" s="4"/>
+      <c r="M79" s="6"/>
+    </row>
+    <row r="80" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D80" s="4"/>
     </row>
-    <row r="81" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="81" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D81" s="4"/>
       <c r="F81" s="4"/>
-      <c r="I81" s="4"/>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
-      <c r="L81" s="6"/>
-    </row>
-    <row r="82" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L81" s="4"/>
+      <c r="M81" s="6"/>
+    </row>
+    <row r="82" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D82" s="4"/>
-      <c r="I82" s="4"/>
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
-      <c r="L82" s="6"/>
-    </row>
-    <row r="83" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L82" s="4"/>
+      <c r="M82" s="6"/>
+    </row>
+    <row r="83" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="84" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D84" s="4"/>
-      <c r="I84" s="4"/>
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
-      <c r="L84" s="6"/>
-    </row>
-    <row r="85" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L84" s="4"/>
+      <c r="M84" s="6"/>
+    </row>
+    <row r="85" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D85" s="4"/>
       <c r="F85" s="4"/>
-      <c r="I85" s="4"/>
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
-      <c r="L85" s="6"/>
-    </row>
-    <row r="86" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L85" s="4"/>
+      <c r="M85" s="6"/>
+    </row>
+    <row r="86" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D86" s="4"/>
-      <c r="I86" s="4"/>
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
-      <c r="L86" s="6"/>
-    </row>
-    <row r="87" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L86" s="4"/>
+      <c r="M86" s="6"/>
+    </row>
+    <row r="87" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="88" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D88" s="4"/>
       <c r="F88" s="4"/>
-      <c r="I88" s="4"/>
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
-      <c r="L88" s="6"/>
-    </row>
-    <row r="89" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L88" s="4"/>
+      <c r="M88" s="6"/>
+    </row>
+    <row r="89" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D89" s="4"/>
-      <c r="I89" s="4"/>
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
-      <c r="L89" s="6"/>
-    </row>
-    <row r="90" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L89" s="4"/>
+      <c r="M89" s="6"/>
+    </row>
+    <row r="90" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D90" s="4"/>
       <c r="F90" s="4"/>
-      <c r="I90" s="4"/>
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
-      <c r="L90" s="6"/>
-    </row>
-    <row r="91" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L90" s="4"/>
+      <c r="M90" s="6"/>
+    </row>
+    <row r="91" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D91" s="4"/>
       <c r="F91" s="4"/>
-      <c r="I91" s="4"/>
       <c r="J91" s="4"/>
       <c r="K91" s="4"/>
-      <c r="L91" s="6"/>
-    </row>
-    <row r="92" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L91" s="4"/>
+      <c r="M91" s="6"/>
+    </row>
+    <row r="92" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D92" s="4"/>
       <c r="F92" s="4"/>
-      <c r="I92" s="4"/>
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
-      <c r="L92" s="6"/>
-    </row>
-    <row r="93" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L92" s="4"/>
+      <c r="M92" s="6"/>
+    </row>
+    <row r="93" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D93" s="4"/>
       <c r="F93" s="4"/>
-      <c r="I93" s="4"/>
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
-      <c r="L93" s="6"/>
-    </row>
-    <row r="94" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L93" s="4"/>
+      <c r="M93" s="6"/>
+    </row>
+    <row r="94" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D94" s="4"/>
-      <c r="I94" s="4"/>
       <c r="J94" s="4"/>
       <c r="K94" s="4"/>
-      <c r="L94" s="6"/>
-    </row>
-    <row r="95" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L94" s="4"/>
+      <c r="M94" s="6"/>
+    </row>
+    <row r="95" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D95" s="4"/>
-      <c r="I95" s="4"/>
       <c r="J95" s="4"/>
       <c r="K95" s="4"/>
-      <c r="L95" s="6"/>
-    </row>
-    <row r="96" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L95" s="4"/>
+      <c r="M95" s="6"/>
+    </row>
+    <row r="96" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D96" s="4"/>
-      <c r="I96" s="4"/>
       <c r="J96" s="4"/>
       <c r="K96" s="4"/>
-      <c r="L96" s="6"/>
-    </row>
-    <row r="97" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L96" s="4"/>
+      <c r="M96" s="6"/>
+    </row>
+    <row r="97" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D97" s="4"/>
       <c r="F97" s="4"/>
-      <c r="I97" s="4"/>
       <c r="J97" s="4"/>
       <c r="K97" s="4"/>
-      <c r="L97" s="6"/>
-    </row>
-    <row r="98" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L97" s="4"/>
+      <c r="M97" s="6"/>
+    </row>
+    <row r="98" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D98" s="4"/>
-      <c r="I98" s="4"/>
       <c r="J98" s="4"/>
       <c r="K98" s="4"/>
-      <c r="L98" s="6"/>
-    </row>
-    <row r="99" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L98" s="4"/>
+      <c r="M98" s="6"/>
+    </row>
+    <row r="99" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D99" s="4"/>
       <c r="F99" s="4"/>
-      <c r="I99" s="4"/>
       <c r="J99" s="4"/>
       <c r="K99" s="4"/>
-      <c r="L99" s="6"/>
-    </row>
-    <row r="100" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L99" s="4"/>
+      <c r="M99" s="6"/>
+    </row>
+    <row r="100" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D100" s="4"/>
       <c r="F100" s="4"/>
-      <c r="I100" s="4"/>
       <c r="J100" s="4"/>
       <c r="K100" s="4"/>
-      <c r="L100" s="6"/>
-    </row>
-    <row r="101" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L100" s="4"/>
+      <c r="M100" s="6"/>
+    </row>
+    <row r="101" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D101" s="4"/>
       <c r="F101" s="4"/>
-      <c r="I101" s="4"/>
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
-      <c r="L101" s="6"/>
-    </row>
-    <row r="102" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L101" s="4"/>
+      <c r="M101" s="6"/>
+    </row>
+    <row r="102" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D102" s="4"/>
       <c r="F102" s="4"/>
-      <c r="I102" s="4"/>
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
-      <c r="L102" s="6"/>
-    </row>
-    <row r="103" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L102" s="4"/>
+      <c r="M102" s="6"/>
+    </row>
+    <row r="103" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D103" s="4"/>
-      <c r="I103" s="4"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
-      <c r="L103" s="6"/>
-    </row>
-    <row r="104" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L103" s="4"/>
+      <c r="M103" s="6"/>
+    </row>
+    <row r="104" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D104" s="4"/>
-      <c r="I104" s="4"/>
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
-      <c r="L104" s="6"/>
-    </row>
-    <row r="105" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L104" s="4"/>
+      <c r="M104" s="6"/>
+    </row>
+    <row r="105" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D105" s="4"/>
       <c r="F105" s="4"/>
-      <c r="I105" s="4"/>
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
-      <c r="L105" s="6"/>
-    </row>
-    <row r="106" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L105" s="4"/>
+      <c r="M105" s="6"/>
+    </row>
+    <row r="106" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D106" s="4"/>
       <c r="F106" s="4"/>
-      <c r="I106" s="4"/>
       <c r="J106" s="4"/>
       <c r="K106" s="4"/>
-      <c r="L106" s="6"/>
-    </row>
-    <row r="107" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L106" s="4"/>
+      <c r="M106" s="6"/>
+    </row>
+    <row r="107" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D107" s="4"/>
-      <c r="I107" s="4"/>
       <c r="J107" s="4"/>
       <c r="K107" s="4"/>
-      <c r="L107" s="6"/>
-    </row>
-    <row r="108" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L107" s="4"/>
+      <c r="M107" s="6"/>
+    </row>
+    <row r="108" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D108" s="4"/>
       <c r="F108" s="4"/>
-      <c r="I108" s="4"/>
       <c r="J108" s="4"/>
       <c r="K108" s="4"/>
-      <c r="L108" s="6"/>
-    </row>
-    <row r="109" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L108" s="4"/>
+      <c r="M108" s="6"/>
+    </row>
+    <row r="109" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D109" s="4"/>
       <c r="F109" s="4"/>
-      <c r="I109" s="4"/>
       <c r="J109" s="4"/>
       <c r="K109" s="4"/>
-      <c r="L109" s="6"/>
-    </row>
-    <row r="110" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L109" s="4"/>
+      <c r="M109" s="6"/>
+    </row>
+    <row r="110" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D110" s="4"/>
-      <c r="I110" s="4"/>
       <c r="J110" s="4"/>
       <c r="K110" s="4"/>
-      <c r="L110" s="6"/>
-    </row>
-    <row r="111" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L110" s="4"/>
+      <c r="M110" s="6"/>
+    </row>
+    <row r="111" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D111" s="4"/>
       <c r="F111" s="4"/>
-      <c r="I111" s="4"/>
       <c r="J111" s="4"/>
       <c r="K111" s="4"/>
-      <c r="L111" s="6"/>
-    </row>
-    <row r="112" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L111" s="4"/>
+      <c r="M111" s="6"/>
+    </row>
+    <row r="112" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D112" s="4"/>
-      <c r="I112" s="4"/>
       <c r="J112" s="4"/>
       <c r="K112" s="4"/>
-      <c r="L112" s="6"/>
-    </row>
-    <row r="113" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L112" s="4"/>
+      <c r="M112" s="6"/>
+    </row>
+    <row r="113" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D113" s="4"/>
-      <c r="I113" s="4"/>
       <c r="J113" s="4"/>
       <c r="K113" s="4"/>
-      <c r="L113" s="6"/>
-    </row>
-    <row r="114" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L113" s="4"/>
+      <c r="M113" s="6"/>
+    </row>
+    <row r="114" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D114" s="4"/>
-      <c r="I114" s="4"/>
       <c r="J114" s="4"/>
       <c r="K114" s="4"/>
-      <c r="L114" s="6"/>
-    </row>
-    <row r="115" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L114" s="4"/>
+      <c r="M114" s="6"/>
+    </row>
+    <row r="115" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D115" s="4"/>
       <c r="F115" s="4"/>
-      <c r="I115" s="4"/>
       <c r="J115" s="4"/>
       <c r="K115" s="4"/>
-      <c r="L115" s="6"/>
-    </row>
-    <row r="116" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L115" s="4"/>
+      <c r="M115" s="6"/>
+    </row>
+    <row r="116" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D116" s="4"/>
       <c r="F116" s="4"/>
-      <c r="I116" s="4"/>
       <c r="J116" s="4"/>
       <c r="K116" s="4"/>
-      <c r="L116" s="6"/>
-    </row>
-    <row r="117" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L116" s="4"/>
+      <c r="M116" s="6"/>
+    </row>
+    <row r="117" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D117" s="4"/>
       <c r="F117" s="4"/>
-      <c r="I117" s="4"/>
       <c r="J117" s="4"/>
       <c r="K117" s="4"/>
-      <c r="L117" s="6"/>
-    </row>
-    <row r="118" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L117" s="4"/>
+      <c r="M117" s="6"/>
+    </row>
+    <row r="118" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D118" s="4"/>
       <c r="F118" s="4"/>
-      <c r="I118" s="4"/>
       <c r="J118" s="4"/>
       <c r="K118" s="4"/>
-      <c r="L118" s="6"/>
-    </row>
-    <row r="119" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L118" s="4"/>
+      <c r="M118" s="6"/>
+    </row>
+    <row r="119" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D119" s="4"/>
       <c r="F119" s="4"/>
-      <c r="I119" s="4"/>
       <c r="J119" s="4"/>
       <c r="K119" s="4"/>
-      <c r="L119" s="6"/>
-    </row>
-    <row r="120" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L119" s="4"/>
+      <c r="M119" s="6"/>
+    </row>
+    <row r="120" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D120" s="4"/>
       <c r="F120" s="4"/>
-      <c r="I120" s="4"/>
       <c r="J120" s="4"/>
       <c r="K120" s="4"/>
-      <c r="L120" s="6"/>
-    </row>
-    <row r="121" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L120" s="4"/>
+      <c r="M120" s="6"/>
+    </row>
+    <row r="121" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D121" s="4"/>
-      <c r="I121" s="4"/>
       <c r="J121" s="4"/>
       <c r="K121" s="4"/>
-      <c r="L121" s="6"/>
-    </row>
-    <row r="122" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L121" s="4"/>
+      <c r="M121" s="6"/>
+    </row>
+    <row r="122" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D122" s="4"/>
-      <c r="I122" s="4"/>
       <c r="J122" s="4"/>
       <c r="K122" s="4"/>
-      <c r="L122" s="6"/>
-    </row>
-    <row r="123" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L122" s="4"/>
+      <c r="M122" s="6"/>
+    </row>
+    <row r="123" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D123" s="4"/>
-      <c r="I123" s="4"/>
       <c r="J123" s="4"/>
       <c r="K123" s="4"/>
-      <c r="L123" s="6"/>
-    </row>
-    <row r="124" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L123" s="4"/>
+      <c r="M123" s="6"/>
+    </row>
+    <row r="124" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D124" s="4"/>
-      <c r="I124" s="4"/>
       <c r="J124" s="4"/>
       <c r="K124" s="4"/>
-      <c r="L124" s="6"/>
-    </row>
-    <row r="125" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L124" s="4"/>
+      <c r="M124" s="6"/>
+    </row>
+    <row r="125" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D125" s="4"/>
-      <c r="I125" s="4"/>
       <c r="J125" s="4"/>
       <c r="K125" s="4"/>
-      <c r="L125" s="6"/>
-    </row>
-    <row r="126" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L125" s="4"/>
+      <c r="M125" s="6"/>
+    </row>
+    <row r="126" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D126" s="4"/>
       <c r="F126" s="4"/>
-      <c r="I126" s="4"/>
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
-      <c r="L126" s="6"/>
-    </row>
-    <row r="127" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L126" s="4"/>
+      <c r="M126" s="6"/>
+    </row>
+    <row r="127" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D127" s="4"/>
-      <c r="I127" s="4"/>
       <c r="J127" s="4"/>
       <c r="K127" s="4"/>
-      <c r="L127" s="6"/>
-    </row>
-    <row r="128" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L127" s="4"/>
+      <c r="M127" s="6"/>
+    </row>
+    <row r="128" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D128" s="4"/>
-      <c r="I128" s="4"/>
       <c r="J128" s="4"/>
       <c r="K128" s="4"/>
-      <c r="L128" s="6"/>
-    </row>
-    <row r="129" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L128" s="4"/>
+      <c r="M128" s="6"/>
+    </row>
+    <row r="129" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="130" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D130" s="4"/>
-      <c r="I130" s="4"/>
       <c r="J130" s="4"/>
       <c r="K130" s="4"/>
-      <c r="L130" s="6"/>
-    </row>
-    <row r="131" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L130" s="4"/>
+      <c r="M130" s="6"/>
+    </row>
+    <row r="131" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="132" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D132" s="4"/>
       <c r="F132" s="4"/>
-      <c r="I132" s="4"/>
       <c r="J132" s="4"/>
       <c r="K132" s="4"/>
-      <c r="L132" s="6"/>
-    </row>
-    <row r="133" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L132" s="4"/>
+      <c r="M132" s="6"/>
+    </row>
+    <row r="133" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D133" s="4"/>
-      <c r="I133" s="4"/>
       <c r="J133" s="4"/>
       <c r="K133" s="4"/>
-      <c r="L133" s="6"/>
-    </row>
-    <row r="134" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L133" s="4"/>
+      <c r="M133" s="6"/>
+    </row>
+    <row r="134" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D134" s="4"/>
-      <c r="I134" s="4"/>
       <c r="J134" s="4"/>
       <c r="K134" s="4"/>
-      <c r="L134" s="6"/>
-    </row>
-    <row r="135" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L134" s="4"/>
+      <c r="M134" s="6"/>
+    </row>
+    <row r="135" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D135" s="4"/>
-      <c r="I135" s="4"/>
       <c r="J135" s="4"/>
       <c r="K135" s="4"/>
-      <c r="L135" s="6"/>
-    </row>
-    <row r="136" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L135" s="4"/>
+      <c r="M135" s="6"/>
+    </row>
+    <row r="136" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D136" s="4"/>
-      <c r="I136" s="4"/>
       <c r="J136" s="4"/>
       <c r="K136" s="4"/>
-      <c r="L136" s="6"/>
-    </row>
-    <row r="137" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L136" s="4"/>
+      <c r="M136" s="6"/>
+    </row>
+    <row r="137" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="138" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="139" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D139" s="4"/>
-      <c r="I139" s="4"/>
       <c r="J139" s="4"/>
       <c r="K139" s="4"/>
-      <c r="L139" s="6"/>
-    </row>
-    <row r="140" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L139" s="4"/>
+      <c r="M139" s="6"/>
+    </row>
+    <row r="140" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D140" s="4"/>
-      <c r="I140" s="4"/>
       <c r="J140" s="4"/>
       <c r="K140" s="4"/>
-      <c r="L140" s="6"/>
-    </row>
-    <row r="141" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L140" s="4"/>
+      <c r="M140" s="6"/>
+    </row>
+    <row r="141" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D141" s="4"/>
-      <c r="I141" s="4"/>
       <c r="J141" s="4"/>
       <c r="K141" s="4"/>
-      <c r="L141" s="6"/>
-    </row>
-    <row r="142" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L141" s="4"/>
+      <c r="M141" s="6"/>
+    </row>
+    <row r="142" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D142" s="4"/>
-      <c r="I142" s="4"/>
       <c r="J142" s="4"/>
       <c r="K142" s="4"/>
-      <c r="L142" s="6"/>
-    </row>
-    <row r="143" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L142" s="4"/>
+      <c r="M142" s="6"/>
+    </row>
+    <row r="143" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D143" s="4"/>
-      <c r="I143" s="4"/>
       <c r="J143" s="4"/>
       <c r="K143" s="4"/>
-      <c r="L143" s="6"/>
-    </row>
-    <row r="144" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L143" s="4"/>
+      <c r="M143" s="6"/>
+    </row>
+    <row r="144" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="145" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D145" s="4"/>
-      <c r="I145" s="4"/>
       <c r="J145" s="4"/>
       <c r="K145" s="4"/>
-      <c r="L145" s="6"/>
-    </row>
-    <row r="146" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L145" s="4"/>
+      <c r="M145" s="6"/>
+    </row>
+    <row r="146" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D146" s="4"/>
-      <c r="I146" s="4"/>
       <c r="J146" s="4"/>
       <c r="K146" s="4"/>
-      <c r="L146" s="6"/>
-    </row>
-    <row r="147" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L146" s="4"/>
+      <c r="M146" s="6"/>
+    </row>
+    <row r="147" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D147" s="4"/>
-      <c r="I147" s="4"/>
       <c r="J147" s="4"/>
       <c r="K147" s="4"/>
-      <c r="L147" s="6"/>
-    </row>
-    <row r="148" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L147" s="4"/>
+      <c r="M147" s="6"/>
+    </row>
+    <row r="148" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D148" s="4"/>
     </row>
-    <row r="149" spans="4:12" x14ac:dyDescent="0.15">
+    <row r="149" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D149" s="4"/>
       <c r="F149" s="4"/>
-      <c r="I149" s="4"/>
       <c r="J149" s="4"/>
       <c r="K149" s="4"/>
-      <c r="L149" s="6"/>
-    </row>
-    <row r="150" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L149" s="4"/>
+      <c r="M149" s="6"/>
+    </row>
+    <row r="150" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D150" s="4"/>
-      <c r="I150" s="4"/>
       <c r="J150" s="4"/>
       <c r="K150" s="4"/>
-      <c r="L150" s="6"/>
-    </row>
-    <row r="151" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L150" s="4"/>
+      <c r="M150" s="6"/>
+    </row>
+    <row r="151" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D151" s="4"/>
-      <c r="I151" s="4"/>
       <c r="J151" s="4"/>
       <c r="K151" s="4"/>
-      <c r="L151" s="6"/>
-    </row>
-    <row r="152" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L151" s="4"/>
+      <c r="M151" s="6"/>
+    </row>
+    <row r="152" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D152" s="4"/>
-      <c r="I152" s="4"/>
       <c r="J152" s="4"/>
       <c r="K152" s="4"/>
-      <c r="L152" s="6"/>
-    </row>
-    <row r="153" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L152" s="4"/>
+      <c r="M152" s="6"/>
+    </row>
+    <row r="153" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D153" s="4"/>
-      <c r="I153" s="4"/>
       <c r="J153" s="4"/>
       <c r="K153" s="4"/>
-      <c r="L153" s="6"/>
-    </row>
-    <row r="154" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L153" s="4"/>
+      <c r="M153" s="6"/>
+    </row>
+    <row r="154" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D154" s="4"/>
-      <c r="I154" s="4"/>
       <c r="J154" s="4"/>
       <c r="K154" s="4"/>
-      <c r="L154" s="6"/>
-    </row>
-    <row r="155" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L154" s="4"/>
+      <c r="M154" s="6"/>
+    </row>
+    <row r="155" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D155" s="4"/>
-      <c r="I155" s="4"/>
       <c r="J155" s="4"/>
       <c r="K155" s="4"/>
-      <c r="L155" s="6"/>
-    </row>
-    <row r="156" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L155" s="4"/>
+      <c r="M155" s="6"/>
+    </row>
+    <row r="156" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D156" s="4"/>
       <c r="F156" s="4"/>
-      <c r="I156" s="4"/>
       <c r="J156" s="4"/>
       <c r="K156" s="4"/>
-      <c r="L156" s="6"/>
-    </row>
-    <row r="157" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L156" s="4"/>
+      <c r="M156" s="6"/>
+    </row>
+    <row r="157" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D157" s="4"/>
       <c r="F157" s="4"/>
-      <c r="I157" s="4"/>
       <c r="J157" s="4"/>
       <c r="K157" s="4"/>
-      <c r="L157" s="6"/>
-    </row>
-    <row r="158" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L157" s="4"/>
+      <c r="M157" s="6"/>
+    </row>
+    <row r="158" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D158" s="4"/>
-      <c r="I158" s="4"/>
       <c r="J158" s="4"/>
       <c r="K158" s="4"/>
-      <c r="L158" s="6"/>
-    </row>
-    <row r="159" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L158" s="4"/>
+      <c r="M158" s="6"/>
+    </row>
+    <row r="159" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D159" s="4"/>
-      <c r="I159" s="4"/>
       <c r="J159" s="4"/>
       <c r="K159" s="4"/>
-      <c r="L159" s="6"/>
-    </row>
-    <row r="160" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L159" s="4"/>
+      <c r="M159" s="6"/>
+    </row>
+    <row r="160" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D160" s="4"/>
       <c r="F160" s="4"/>
-      <c r="I160" s="4"/>
       <c r="J160" s="4"/>
       <c r="K160" s="4"/>
-      <c r="L160" s="6"/>
-    </row>
-    <row r="161" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L160" s="4"/>
+      <c r="M160" s="6"/>
+    </row>
+    <row r="161" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D161" s="4"/>
       <c r="F161" s="4"/>
-      <c r="I161" s="4"/>
       <c r="J161" s="4"/>
       <c r="K161" s="4"/>
-      <c r="L161" s="6"/>
-    </row>
-    <row r="162" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L161" s="4"/>
+      <c r="M161" s="6"/>
+    </row>
+    <row r="162" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D162" s="4"/>
-      <c r="I162" s="4"/>
       <c r="J162" s="4"/>
       <c r="K162" s="4"/>
-      <c r="L162" s="6"/>
-    </row>
-    <row r="163" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L162" s="4"/>
+      <c r="M162" s="6"/>
+    </row>
+    <row r="163" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D163" s="4"/>
-      <c r="I163" s="4"/>
       <c r="J163" s="4"/>
       <c r="K163" s="4"/>
-      <c r="L163" s="6"/>
-    </row>
-    <row r="164" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L163" s="4"/>
+      <c r="M163" s="6"/>
+    </row>
+    <row r="164" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D164" s="4"/>
       <c r="F164" s="4"/>
-      <c r="I164" s="4"/>
       <c r="J164" s="4"/>
       <c r="K164" s="4"/>
-      <c r="L164" s="6"/>
-    </row>
-    <row r="165" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L164" s="4"/>
+      <c r="M164" s="6"/>
+    </row>
+    <row r="165" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D165" s="4"/>
-      <c r="I165" s="4"/>
       <c r="J165" s="4"/>
       <c r="K165" s="4"/>
-      <c r="L165" s="6"/>
-    </row>
-    <row r="166" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L165" s="4"/>
+      <c r="M165" s="6"/>
+    </row>
+    <row r="166" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D166" s="4"/>
-      <c r="I166" s="4"/>
       <c r="J166" s="4"/>
       <c r="K166" s="4"/>
-      <c r="L166" s="6"/>
-    </row>
-    <row r="167" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L166" s="4"/>
+      <c r="M166" s="6"/>
+    </row>
+    <row r="167" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D167" s="4"/>
-      <c r="I167" s="4"/>
       <c r="J167" s="4"/>
       <c r="K167" s="4"/>
-      <c r="L167" s="6"/>
-    </row>
-    <row r="168" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L167" s="4"/>
+      <c r="M167" s="6"/>
+    </row>
+    <row r="168" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D168" s="4"/>
-      <c r="I168" s="4"/>
       <c r="J168" s="4"/>
       <c r="K168" s="4"/>
-      <c r="L168" s="6"/>
-    </row>
-    <row r="169" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L168" s="4"/>
+      <c r="M168" s="6"/>
+    </row>
+    <row r="169" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D169" s="4"/>
-      <c r="I169" s="4"/>
       <c r="J169" s="4"/>
       <c r="K169" s="4"/>
-      <c r="L169" s="6"/>
-    </row>
-    <row r="170" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L169" s="4"/>
+      <c r="M169" s="6"/>
+    </row>
+    <row r="170" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D170" s="4"/>
-      <c r="I170" s="4"/>
       <c r="J170" s="4"/>
       <c r="K170" s="4"/>
-      <c r="L170" s="6"/>
-    </row>
-    <row r="171" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L170" s="4"/>
+      <c r="M170" s="6"/>
+    </row>
+    <row r="171" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D171" s="4"/>
-      <c r="I171" s="4"/>
       <c r="J171" s="4"/>
       <c r="K171" s="4"/>
-      <c r="L171" s="6"/>
-    </row>
-    <row r="172" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L171" s="4"/>
+      <c r="M171" s="6"/>
+    </row>
+    <row r="172" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D172" s="4"/>
-      <c r="I172" s="4"/>
       <c r="J172" s="4"/>
       <c r="K172" s="4"/>
-      <c r="L172" s="6"/>
-    </row>
-    <row r="173" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L172" s="4"/>
+      <c r="M172" s="6"/>
+    </row>
+    <row r="173" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D173" s="4"/>
-      <c r="I173" s="4"/>
       <c r="J173" s="4"/>
       <c r="K173" s="4"/>
-      <c r="L173" s="6"/>
-    </row>
-    <row r="174" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L173" s="4"/>
+      <c r="M173" s="6"/>
+    </row>
+    <row r="174" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D174" s="4"/>
-      <c r="I174" s="4"/>
       <c r="J174" s="4"/>
       <c r="K174" s="4"/>
-      <c r="L174" s="6"/>
-    </row>
-    <row r="175" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L174" s="4"/>
+      <c r="M174" s="6"/>
+    </row>
+    <row r="175" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D175" s="4"/>
-      <c r="I175" s="4"/>
       <c r="J175" s="4"/>
       <c r="K175" s="4"/>
-      <c r="L175" s="6"/>
-    </row>
-    <row r="176" spans="4:12" x14ac:dyDescent="0.15">
+      <c r="L175" s="4"/>
+      <c r="M175" s="6"/>
+    </row>
+    <row r="176" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D176" s="4"/>
       <c r="F176" s="4"/>
-      <c r="I176" s="4"/>
       <c r="J176" s="4"/>
       <c r="K176" s="4"/>
-      <c r="L176" s="6"/>
-    </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="L176" s="4"/>
+      <c r="M176" s="6"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D177" s="4"/>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D178" s="4"/>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D179" s="4"/>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D180" s="4"/>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D181" s="4"/>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D182" s="4"/>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D183" s="4"/>
     </row>
   </sheetData>
@@ -2050,51 +2049,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="8" customWidth="1"/>
-    <col min="2" max="3" width="25.5" style="8" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="8" customWidth="1"/>
+    <col min="2" max="3" width="25.42578125" style="8" customWidth="1"/>
     <col min="4" max="4" width="62" style="8" customWidth="1"/>
-    <col min="5" max="5" width="25.5" style="8" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
-    <col min="7" max="7" width="67.1640625" style="8" customWidth="1"/>
-    <col min="8" max="1020" width="11.5" style="8"/>
-    <col min="1021" max="1022" width="8.6640625" style="7" customWidth="1"/>
-    <col min="1023" max="16384" width="9.1640625" style="7"/>
+    <col min="5" max="5" width="25.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="67.140625" style="8" customWidth="1"/>
+    <col min="8" max="1020" width="11.42578125" style="8"/>
+    <col min="1021" max="1022" width="8.7109375" style="7" customWidth="1"/>
+    <col min="1023" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1024" s="14" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="AMG1" s="15"/>
       <c r="AMH1" s="15"/>

</xml_diff>

<commit_message>
fix: chiffres de la dom
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CD8FC5-FDB9-B749-8BE2-8C2FBACB2468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AA5D07-3199-0A4E-9D61-85EF3088E633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23220" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23220" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats Globales" sheetId="1" r:id="rId1"/>
     <sheet name="Liste Structures" sheetId="2" r:id="rId2"/>
     <sheet name="Liste utilisateurs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>Date et heure</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Structures</t>
-  </si>
-  <si>
-    <t>Tous</t>
   </si>
   <si>
     <t>Actifs</t>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>Domiciliés</t>
+  </si>
+  <si>
+    <t>Ayants-droits</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -606,7 +606,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="9"/>
       <c r="D4" s="9"/>
@@ -614,7 +614,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="9"/>
       <c r="D5" s="9"/>
@@ -622,7 +622,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="9"/>
       <c r="D6" s="9"/>
@@ -630,7 +630,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="9"/>
       <c r="D7" s="9"/>
@@ -638,7 +638,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="9"/>
       <c r="D8" s="9"/>
@@ -646,7 +646,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="9"/>
       <c r="D9" s="9"/>
@@ -654,7 +654,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="12"/>
       <c r="D10" s="12"/>
@@ -673,7 +673,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="9"/>
       <c r="D13" s="12"/>
@@ -681,7 +681,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="9"/>
       <c r="D14" s="12"/>
@@ -689,7 +689,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="9"/>
       <c r="D15" s="12"/>
@@ -697,7 +697,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="9"/>
       <c r="D16" s="12"/>
@@ -709,7 +709,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="9"/>
       <c r="D18" s="9"/>
@@ -717,66 +717,66 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="12"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="9"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="9"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="12"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="9"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="9"/>
     </row>
@@ -788,11 +788,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AML183"/>
+  <dimension ref="A1:AMM183"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -804,1226 +804,1229 @@
     <col min="5" max="5" width="11.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="5" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" style="3" customWidth="1"/>
-    <col min="8" max="9" width="12.5" style="3" customWidth="1"/>
-    <col min="10" max="11" width="13" style="5" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="33" style="3" customWidth="1"/>
-    <col min="14" max="14" width="7.83203125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="35" style="3" customWidth="1"/>
-    <col min="16" max="16" width="44.33203125" style="3" customWidth="1"/>
-    <col min="17" max="1026" width="8.6640625" style="3" customWidth="1"/>
-    <col min="1027" max="16384" width="9.1640625" style="7"/>
+    <col min="8" max="10" width="12.5" style="3" customWidth="1"/>
+    <col min="11" max="12" width="13" style="5" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="33" style="3" customWidth="1"/>
+    <col min="15" max="15" width="7.83203125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="35" style="3" customWidth="1"/>
+    <col min="17" max="17" width="44.33203125" style="3" customWidth="1"/>
+    <col min="18" max="1027" width="8.6640625" style="3" customWidth="1"/>
+    <col min="1028" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M2" s="4"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D3" s="4"/>
-      <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M3" s="4"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D4" s="4"/>
-      <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M4" s="4"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D5" s="4"/>
-      <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M5" s="4"/>
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D6" s="4"/>
-      <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M6" s="4"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D7" s="4"/>
-      <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M7" s="4"/>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D8" s="4"/>
-      <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M8" s="4"/>
+      <c r="N8" s="6"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D9" s="4"/>
-      <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M9" s="4"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D10" s="4"/>
-      <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M10" s="4"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D11" s="4"/>
-      <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M11" s="4"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D12" s="4"/>
-      <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M12" s="4"/>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D13" s="4"/>
-      <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M13" s="4"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D14" s="4"/>
-      <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M14" s="4"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D15" s="4"/>
-      <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M15" s="4"/>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D17" s="4"/>
-      <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M17" s="4"/>
+      <c r="N17" s="6"/>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D18" s="4"/>
-      <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="6"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M18" s="4"/>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D19" s="4"/>
-      <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M19" s="4"/>
+      <c r="N19" s="6"/>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D20" s="4"/>
-      <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M20" s="4"/>
+      <c r="N20" s="6"/>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D21" s="4"/>
-      <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="6"/>
-    </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M21" s="4"/>
+      <c r="N21" s="6"/>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D22" s="4"/>
-      <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M22" s="4"/>
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D23" s="4"/>
-      <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="6"/>
-    </row>
-    <row r="24" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M23" s="4"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M24" s="4"/>
+      <c r="N24" s="6"/>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="26" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M26" s="4"/>
+      <c r="N26" s="6"/>
+    </row>
+    <row r="27" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D27" s="4"/>
-      <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="6"/>
-    </row>
-    <row r="28" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M27" s="4"/>
+      <c r="N27" s="6"/>
+    </row>
+    <row r="28" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D28" s="4"/>
-      <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="6"/>
-    </row>
-    <row r="29" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M28" s="4"/>
+      <c r="N28" s="6"/>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="6"/>
-    </row>
-    <row r="30" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M29" s="4"/>
+      <c r="N29" s="6"/>
+    </row>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D30" s="4"/>
-      <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="6"/>
-    </row>
-    <row r="31" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M30" s="4"/>
+      <c r="N30" s="6"/>
+    </row>
+    <row r="31" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D31" s="4"/>
-      <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="6"/>
-    </row>
-    <row r="32" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M31" s="4"/>
+      <c r="N31" s="6"/>
+    </row>
+    <row r="32" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D32" s="4"/>
-      <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="6"/>
-    </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M32" s="4"/>
+      <c r="N32" s="6"/>
+    </row>
+    <row r="33" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D33" s="4"/>
-      <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="6"/>
-    </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M33" s="4"/>
+      <c r="N33" s="6"/>
+    </row>
+    <row r="34" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D34" s="4"/>
-      <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="M34" s="6"/>
-    </row>
-    <row r="35" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M34" s="4"/>
+      <c r="N34" s="6"/>
+    </row>
+    <row r="35" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="36" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="37" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D37" s="4"/>
-      <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="6"/>
-    </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M37" s="4"/>
+      <c r="N37" s="6"/>
+    </row>
+    <row r="38" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="39" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D39" s="4"/>
-      <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="6"/>
-    </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M39" s="4"/>
+      <c r="N39" s="6"/>
+    </row>
+    <row r="40" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D40" s="4"/>
-      <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="6"/>
-    </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M40" s="4"/>
+      <c r="N40" s="6"/>
+    </row>
+    <row r="41" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D41" s="4"/>
-      <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="6"/>
-    </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M41" s="4"/>
+      <c r="N41" s="6"/>
+    </row>
+    <row r="42" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
-      <c r="M42" s="6"/>
-    </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M42" s="4"/>
+      <c r="N42" s="6"/>
+    </row>
+    <row r="43" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="6"/>
-    </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M43" s="4"/>
+      <c r="N43" s="6"/>
+    </row>
+    <row r="44" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="6"/>
-    </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M44" s="4"/>
+      <c r="N44" s="6"/>
+    </row>
+    <row r="45" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D45" s="4"/>
-      <c r="J45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
-      <c r="M45" s="6"/>
-    </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M45" s="4"/>
+      <c r="N45" s="6"/>
+    </row>
+    <row r="46" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="47" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="48" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="49" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D49" s="4"/>
-      <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="6"/>
-    </row>
-    <row r="50" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M49" s="4"/>
+      <c r="N49" s="6"/>
+    </row>
+    <row r="50" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="51" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="52" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D52" s="4"/>
-      <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="6"/>
-    </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M52" s="4"/>
+      <c r="N52" s="6"/>
+    </row>
+    <row r="53" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D53" s="4"/>
       <c r="F53" s="4"/>
-      <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="6"/>
-    </row>
-    <row r="54" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M53" s="4"/>
+      <c r="N53" s="6"/>
+    </row>
+    <row r="54" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="55" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="56" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="57" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
-      <c r="M57" s="6"/>
-    </row>
-    <row r="58" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M57" s="4"/>
+      <c r="N57" s="6"/>
+    </row>
+    <row r="58" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
-      <c r="M58" s="6"/>
-    </row>
-    <row r="59" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M58" s="4"/>
+      <c r="N58" s="6"/>
+    </row>
+    <row r="59" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="60" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D60" s="4"/>
       <c r="F60" s="4"/>
-      <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
-      <c r="M60" s="6"/>
-    </row>
-    <row r="61" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M60" s="4"/>
+      <c r="N60" s="6"/>
+    </row>
+    <row r="61" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D61" s="4"/>
-      <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
-      <c r="M61" s="6"/>
-    </row>
-    <row r="62" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M61" s="4"/>
+      <c r="N61" s="6"/>
+    </row>
+    <row r="62" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D62" s="4"/>
-      <c r="J62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
-      <c r="M62" s="6"/>
-    </row>
-    <row r="63" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M62" s="4"/>
+      <c r="N62" s="6"/>
+    </row>
+    <row r="63" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="64" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D64" s="4"/>
-      <c r="J64" s="4"/>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
-      <c r="M64" s="6"/>
-    </row>
-    <row r="65" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M64" s="4"/>
+      <c r="N64" s="6"/>
+    </row>
+    <row r="65" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="66" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D66" s="4"/>
       <c r="F66" s="4"/>
-      <c r="J66" s="4"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
-      <c r="M66" s="6"/>
-    </row>
-    <row r="67" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M66" s="4"/>
+      <c r="N66" s="6"/>
+    </row>
+    <row r="67" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D67" s="4"/>
-      <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
-      <c r="M67" s="6"/>
-    </row>
-    <row r="68" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M67" s="4"/>
+      <c r="N67" s="6"/>
+    </row>
+    <row r="68" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D68" s="4"/>
-      <c r="J68" s="4"/>
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
-      <c r="M68" s="6"/>
-    </row>
-    <row r="69" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M68" s="4"/>
+      <c r="N68" s="6"/>
+    </row>
+    <row r="69" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D69" s="4"/>
-      <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="6"/>
-    </row>
-    <row r="70" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M69" s="4"/>
+      <c r="N69" s="6"/>
+    </row>
+    <row r="70" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D70" s="4"/>
-      <c r="J70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
-      <c r="M70" s="6"/>
-    </row>
-    <row r="71" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M70" s="4"/>
+      <c r="N70" s="6"/>
+    </row>
+    <row r="71" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D71" s="4"/>
-      <c r="J71" s="4"/>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
-      <c r="M71" s="6"/>
-    </row>
-    <row r="72" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M71" s="4"/>
+      <c r="N71" s="6"/>
+    </row>
+    <row r="72" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D72" s="4"/>
       <c r="F72" s="4"/>
-      <c r="J72" s="4"/>
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
-      <c r="M72" s="6"/>
-    </row>
-    <row r="73" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M72" s="4"/>
+      <c r="N72" s="6"/>
+    </row>
+    <row r="73" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="74" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D74" s="4"/>
-      <c r="J74" s="4"/>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
-      <c r="M74" s="6"/>
-    </row>
-    <row r="75" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M74" s="4"/>
+      <c r="N74" s="6"/>
+    </row>
+    <row r="75" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D75" s="4"/>
       <c r="F75" s="4"/>
-      <c r="J75" s="4"/>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
-      <c r="M75" s="6"/>
-    </row>
-    <row r="76" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M75" s="4"/>
+      <c r="N75" s="6"/>
+    </row>
+    <row r="76" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="77" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D77" s="4"/>
       <c r="F77" s="4"/>
-      <c r="J77" s="4"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
-      <c r="M77" s="6"/>
-    </row>
-    <row r="78" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M77" s="4"/>
+      <c r="N77" s="6"/>
+    </row>
+    <row r="78" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="79" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D79" s="4"/>
-      <c r="J79" s="4"/>
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
-      <c r="M79" s="6"/>
-    </row>
-    <row r="80" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M79" s="4"/>
+      <c r="N79" s="6"/>
+    </row>
+    <row r="80" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D80" s="4"/>
     </row>
-    <row r="81" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="81" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D81" s="4"/>
       <c r="F81" s="4"/>
-      <c r="J81" s="4"/>
       <c r="K81" s="4"/>
       <c r="L81" s="4"/>
-      <c r="M81" s="6"/>
-    </row>
-    <row r="82" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M81" s="4"/>
+      <c r="N81" s="6"/>
+    </row>
+    <row r="82" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D82" s="4"/>
-      <c r="J82" s="4"/>
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
-      <c r="M82" s="6"/>
-    </row>
-    <row r="83" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M82" s="4"/>
+      <c r="N82" s="6"/>
+    </row>
+    <row r="83" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="84" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D84" s="4"/>
-      <c r="J84" s="4"/>
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
-      <c r="M84" s="6"/>
-    </row>
-    <row r="85" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M84" s="4"/>
+      <c r="N84" s="6"/>
+    </row>
+    <row r="85" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D85" s="4"/>
       <c r="F85" s="4"/>
-      <c r="J85" s="4"/>
       <c r="K85" s="4"/>
       <c r="L85" s="4"/>
-      <c r="M85" s="6"/>
-    </row>
-    <row r="86" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M85" s="4"/>
+      <c r="N85" s="6"/>
+    </row>
+    <row r="86" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D86" s="4"/>
-      <c r="J86" s="4"/>
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
-      <c r="M86" s="6"/>
-    </row>
-    <row r="87" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M86" s="4"/>
+      <c r="N86" s="6"/>
+    </row>
+    <row r="87" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="88" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D88" s="4"/>
       <c r="F88" s="4"/>
-      <c r="J88" s="4"/>
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
-      <c r="M88" s="6"/>
-    </row>
-    <row r="89" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M88" s="4"/>
+      <c r="N88" s="6"/>
+    </row>
+    <row r="89" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D89" s="4"/>
-      <c r="J89" s="4"/>
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
-      <c r="M89" s="6"/>
-    </row>
-    <row r="90" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M89" s="4"/>
+      <c r="N89" s="6"/>
+    </row>
+    <row r="90" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D90" s="4"/>
       <c r="F90" s="4"/>
-      <c r="J90" s="4"/>
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
-      <c r="M90" s="6"/>
-    </row>
-    <row r="91" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M90" s="4"/>
+      <c r="N90" s="6"/>
+    </row>
+    <row r="91" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D91" s="4"/>
       <c r="F91" s="4"/>
-      <c r="J91" s="4"/>
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
-      <c r="M91" s="6"/>
-    </row>
-    <row r="92" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M91" s="4"/>
+      <c r="N91" s="6"/>
+    </row>
+    <row r="92" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D92" s="4"/>
       <c r="F92" s="4"/>
-      <c r="J92" s="4"/>
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
-      <c r="M92" s="6"/>
-    </row>
-    <row r="93" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M92" s="4"/>
+      <c r="N92" s="6"/>
+    </row>
+    <row r="93" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D93" s="4"/>
       <c r="F93" s="4"/>
-      <c r="J93" s="4"/>
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
-      <c r="M93" s="6"/>
-    </row>
-    <row r="94" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M93" s="4"/>
+      <c r="N93" s="6"/>
+    </row>
+    <row r="94" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D94" s="4"/>
-      <c r="J94" s="4"/>
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
-      <c r="M94" s="6"/>
-    </row>
-    <row r="95" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M94" s="4"/>
+      <c r="N94" s="6"/>
+    </row>
+    <row r="95" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D95" s="4"/>
-      <c r="J95" s="4"/>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
-      <c r="M95" s="6"/>
-    </row>
-    <row r="96" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M95" s="4"/>
+      <c r="N95" s="6"/>
+    </row>
+    <row r="96" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D96" s="4"/>
-      <c r="J96" s="4"/>
       <c r="K96" s="4"/>
       <c r="L96" s="4"/>
-      <c r="M96" s="6"/>
-    </row>
-    <row r="97" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M96" s="4"/>
+      <c r="N96" s="6"/>
+    </row>
+    <row r="97" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D97" s="4"/>
       <c r="F97" s="4"/>
-      <c r="J97" s="4"/>
       <c r="K97" s="4"/>
       <c r="L97" s="4"/>
-      <c r="M97" s="6"/>
-    </row>
-    <row r="98" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M97" s="4"/>
+      <c r="N97" s="6"/>
+    </row>
+    <row r="98" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D98" s="4"/>
-      <c r="J98" s="4"/>
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
-      <c r="M98" s="6"/>
-    </row>
-    <row r="99" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M98" s="4"/>
+      <c r="N98" s="6"/>
+    </row>
+    <row r="99" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D99" s="4"/>
       <c r="F99" s="4"/>
-      <c r="J99" s="4"/>
       <c r="K99" s="4"/>
       <c r="L99" s="4"/>
-      <c r="M99" s="6"/>
-    </row>
-    <row r="100" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M99" s="4"/>
+      <c r="N99" s="6"/>
+    </row>
+    <row r="100" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D100" s="4"/>
       <c r="F100" s="4"/>
-      <c r="J100" s="4"/>
       <c r="K100" s="4"/>
       <c r="L100" s="4"/>
-      <c r="M100" s="6"/>
-    </row>
-    <row r="101" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M100" s="4"/>
+      <c r="N100" s="6"/>
+    </row>
+    <row r="101" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D101" s="4"/>
       <c r="F101" s="4"/>
-      <c r="J101" s="4"/>
       <c r="K101" s="4"/>
       <c r="L101" s="4"/>
-      <c r="M101" s="6"/>
-    </row>
-    <row r="102" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M101" s="4"/>
+      <c r="N101" s="6"/>
+    </row>
+    <row r="102" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D102" s="4"/>
       <c r="F102" s="4"/>
-      <c r="J102" s="4"/>
       <c r="K102" s="4"/>
       <c r="L102" s="4"/>
-      <c r="M102" s="6"/>
-    </row>
-    <row r="103" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M102" s="4"/>
+      <c r="N102" s="6"/>
+    </row>
+    <row r="103" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D103" s="4"/>
-      <c r="J103" s="4"/>
       <c r="K103" s="4"/>
       <c r="L103" s="4"/>
-      <c r="M103" s="6"/>
-    </row>
-    <row r="104" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M103" s="4"/>
+      <c r="N103" s="6"/>
+    </row>
+    <row r="104" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D104" s="4"/>
-      <c r="J104" s="4"/>
       <c r="K104" s="4"/>
       <c r="L104" s="4"/>
-      <c r="M104" s="6"/>
-    </row>
-    <row r="105" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M104" s="4"/>
+      <c r="N104" s="6"/>
+    </row>
+    <row r="105" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D105" s="4"/>
       <c r="F105" s="4"/>
-      <c r="J105" s="4"/>
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
-      <c r="M105" s="6"/>
-    </row>
-    <row r="106" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M105" s="4"/>
+      <c r="N105" s="6"/>
+    </row>
+    <row r="106" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D106" s="4"/>
       <c r="F106" s="4"/>
-      <c r="J106" s="4"/>
       <c r="K106" s="4"/>
       <c r="L106" s="4"/>
-      <c r="M106" s="6"/>
-    </row>
-    <row r="107" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M106" s="4"/>
+      <c r="N106" s="6"/>
+    </row>
+    <row r="107" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D107" s="4"/>
-      <c r="J107" s="4"/>
       <c r="K107" s="4"/>
       <c r="L107" s="4"/>
-      <c r="M107" s="6"/>
-    </row>
-    <row r="108" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M107" s="4"/>
+      <c r="N107" s="6"/>
+    </row>
+    <row r="108" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D108" s="4"/>
       <c r="F108" s="4"/>
-      <c r="J108" s="4"/>
       <c r="K108" s="4"/>
       <c r="L108" s="4"/>
-      <c r="M108" s="6"/>
-    </row>
-    <row r="109" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M108" s="4"/>
+      <c r="N108" s="6"/>
+    </row>
+    <row r="109" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D109" s="4"/>
       <c r="F109" s="4"/>
-      <c r="J109" s="4"/>
       <c r="K109" s="4"/>
       <c r="L109" s="4"/>
-      <c r="M109" s="6"/>
-    </row>
-    <row r="110" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M109" s="4"/>
+      <c r="N109" s="6"/>
+    </row>
+    <row r="110" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D110" s="4"/>
-      <c r="J110" s="4"/>
       <c r="K110" s="4"/>
       <c r="L110" s="4"/>
-      <c r="M110" s="6"/>
-    </row>
-    <row r="111" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M110" s="4"/>
+      <c r="N110" s="6"/>
+    </row>
+    <row r="111" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D111" s="4"/>
       <c r="F111" s="4"/>
-      <c r="J111" s="4"/>
       <c r="K111" s="4"/>
       <c r="L111" s="4"/>
-      <c r="M111" s="6"/>
-    </row>
-    <row r="112" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M111" s="4"/>
+      <c r="N111" s="6"/>
+    </row>
+    <row r="112" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D112" s="4"/>
-      <c r="J112" s="4"/>
       <c r="K112" s="4"/>
       <c r="L112" s="4"/>
-      <c r="M112" s="6"/>
-    </row>
-    <row r="113" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M112" s="4"/>
+      <c r="N112" s="6"/>
+    </row>
+    <row r="113" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D113" s="4"/>
-      <c r="J113" s="4"/>
       <c r="K113" s="4"/>
       <c r="L113" s="4"/>
-      <c r="M113" s="6"/>
-    </row>
-    <row r="114" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M113" s="4"/>
+      <c r="N113" s="6"/>
+    </row>
+    <row r="114" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D114" s="4"/>
-      <c r="J114" s="4"/>
       <c r="K114" s="4"/>
       <c r="L114" s="4"/>
-      <c r="M114" s="6"/>
-    </row>
-    <row r="115" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M114" s="4"/>
+      <c r="N114" s="6"/>
+    </row>
+    <row r="115" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D115" s="4"/>
       <c r="F115" s="4"/>
-      <c r="J115" s="4"/>
       <c r="K115" s="4"/>
       <c r="L115" s="4"/>
-      <c r="M115" s="6"/>
-    </row>
-    <row r="116" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M115" s="4"/>
+      <c r="N115" s="6"/>
+    </row>
+    <row r="116" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D116" s="4"/>
       <c r="F116" s="4"/>
-      <c r="J116" s="4"/>
       <c r="K116" s="4"/>
       <c r="L116" s="4"/>
-      <c r="M116" s="6"/>
-    </row>
-    <row r="117" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M116" s="4"/>
+      <c r="N116" s="6"/>
+    </row>
+    <row r="117" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D117" s="4"/>
       <c r="F117" s="4"/>
-      <c r="J117" s="4"/>
       <c r="K117" s="4"/>
       <c r="L117" s="4"/>
-      <c r="M117" s="6"/>
-    </row>
-    <row r="118" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M117" s="4"/>
+      <c r="N117" s="6"/>
+    </row>
+    <row r="118" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D118" s="4"/>
       <c r="F118" s="4"/>
-      <c r="J118" s="4"/>
       <c r="K118" s="4"/>
       <c r="L118" s="4"/>
-      <c r="M118" s="6"/>
-    </row>
-    <row r="119" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M118" s="4"/>
+      <c r="N118" s="6"/>
+    </row>
+    <row r="119" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D119" s="4"/>
       <c r="F119" s="4"/>
-      <c r="J119" s="4"/>
       <c r="K119" s="4"/>
       <c r="L119" s="4"/>
-      <c r="M119" s="6"/>
-    </row>
-    <row r="120" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M119" s="4"/>
+      <c r="N119" s="6"/>
+    </row>
+    <row r="120" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D120" s="4"/>
       <c r="F120" s="4"/>
-      <c r="J120" s="4"/>
       <c r="K120" s="4"/>
       <c r="L120" s="4"/>
-      <c r="M120" s="6"/>
-    </row>
-    <row r="121" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M120" s="4"/>
+      <c r="N120" s="6"/>
+    </row>
+    <row r="121" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D121" s="4"/>
-      <c r="J121" s="4"/>
       <c r="K121" s="4"/>
       <c r="L121" s="4"/>
-      <c r="M121" s="6"/>
-    </row>
-    <row r="122" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M121" s="4"/>
+      <c r="N121" s="6"/>
+    </row>
+    <row r="122" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D122" s="4"/>
-      <c r="J122" s="4"/>
       <c r="K122" s="4"/>
       <c r="L122" s="4"/>
-      <c r="M122" s="6"/>
-    </row>
-    <row r="123" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M122" s="4"/>
+      <c r="N122" s="6"/>
+    </row>
+    <row r="123" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D123" s="4"/>
-      <c r="J123" s="4"/>
       <c r="K123" s="4"/>
       <c r="L123" s="4"/>
-      <c r="M123" s="6"/>
-    </row>
-    <row r="124" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M123" s="4"/>
+      <c r="N123" s="6"/>
+    </row>
+    <row r="124" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D124" s="4"/>
-      <c r="J124" s="4"/>
       <c r="K124" s="4"/>
       <c r="L124" s="4"/>
-      <c r="M124" s="6"/>
-    </row>
-    <row r="125" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M124" s="4"/>
+      <c r="N124" s="6"/>
+    </row>
+    <row r="125" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D125" s="4"/>
-      <c r="J125" s="4"/>
       <c r="K125" s="4"/>
       <c r="L125" s="4"/>
-      <c r="M125" s="6"/>
-    </row>
-    <row r="126" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M125" s="4"/>
+      <c r="N125" s="6"/>
+    </row>
+    <row r="126" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D126" s="4"/>
       <c r="F126" s="4"/>
-      <c r="J126" s="4"/>
       <c r="K126" s="4"/>
       <c r="L126" s="4"/>
-      <c r="M126" s="6"/>
-    </row>
-    <row r="127" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M126" s="4"/>
+      <c r="N126" s="6"/>
+    </row>
+    <row r="127" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D127" s="4"/>
-      <c r="J127" s="4"/>
       <c r="K127" s="4"/>
       <c r="L127" s="4"/>
-      <c r="M127" s="6"/>
-    </row>
-    <row r="128" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M127" s="4"/>
+      <c r="N127" s="6"/>
+    </row>
+    <row r="128" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D128" s="4"/>
-      <c r="J128" s="4"/>
       <c r="K128" s="4"/>
       <c r="L128" s="4"/>
-      <c r="M128" s="6"/>
-    </row>
-    <row r="129" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M128" s="4"/>
+      <c r="N128" s="6"/>
+    </row>
+    <row r="129" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="130" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D130" s="4"/>
-      <c r="J130" s="4"/>
       <c r="K130" s="4"/>
       <c r="L130" s="4"/>
-      <c r="M130" s="6"/>
-    </row>
-    <row r="131" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M130" s="4"/>
+      <c r="N130" s="6"/>
+    </row>
+    <row r="131" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="132" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D132" s="4"/>
       <c r="F132" s="4"/>
-      <c r="J132" s="4"/>
       <c r="K132" s="4"/>
       <c r="L132" s="4"/>
-      <c r="M132" s="6"/>
-    </row>
-    <row r="133" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M132" s="4"/>
+      <c r="N132" s="6"/>
+    </row>
+    <row r="133" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D133" s="4"/>
-      <c r="J133" s="4"/>
       <c r="K133" s="4"/>
       <c r="L133" s="4"/>
-      <c r="M133" s="6"/>
-    </row>
-    <row r="134" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M133" s="4"/>
+      <c r="N133" s="6"/>
+    </row>
+    <row r="134" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D134" s="4"/>
-      <c r="J134" s="4"/>
       <c r="K134" s="4"/>
       <c r="L134" s="4"/>
-      <c r="M134" s="6"/>
-    </row>
-    <row r="135" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M134" s="4"/>
+      <c r="N134" s="6"/>
+    </row>
+    <row r="135" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D135" s="4"/>
-      <c r="J135" s="4"/>
       <c r="K135" s="4"/>
       <c r="L135" s="4"/>
-      <c r="M135" s="6"/>
-    </row>
-    <row r="136" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M135" s="4"/>
+      <c r="N135" s="6"/>
+    </row>
+    <row r="136" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D136" s="4"/>
-      <c r="J136" s="4"/>
       <c r="K136" s="4"/>
       <c r="L136" s="4"/>
-      <c r="M136" s="6"/>
-    </row>
-    <row r="137" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M136" s="4"/>
+      <c r="N136" s="6"/>
+    </row>
+    <row r="137" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="138" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="139" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D139" s="4"/>
-      <c r="J139" s="4"/>
       <c r="K139" s="4"/>
       <c r="L139" s="4"/>
-      <c r="M139" s="6"/>
-    </row>
-    <row r="140" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M139" s="4"/>
+      <c r="N139" s="6"/>
+    </row>
+    <row r="140" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D140" s="4"/>
-      <c r="J140" s="4"/>
       <c r="K140" s="4"/>
       <c r="L140" s="4"/>
-      <c r="M140" s="6"/>
-    </row>
-    <row r="141" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M140" s="4"/>
+      <c r="N140" s="6"/>
+    </row>
+    <row r="141" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D141" s="4"/>
-      <c r="J141" s="4"/>
       <c r="K141" s="4"/>
       <c r="L141" s="4"/>
-      <c r="M141" s="6"/>
-    </row>
-    <row r="142" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M141" s="4"/>
+      <c r="N141" s="6"/>
+    </row>
+    <row r="142" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D142" s="4"/>
-      <c r="J142" s="4"/>
       <c r="K142" s="4"/>
       <c r="L142" s="4"/>
-      <c r="M142" s="6"/>
-    </row>
-    <row r="143" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M142" s="4"/>
+      <c r="N142" s="6"/>
+    </row>
+    <row r="143" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D143" s="4"/>
-      <c r="J143" s="4"/>
       <c r="K143" s="4"/>
       <c r="L143" s="4"/>
-      <c r="M143" s="6"/>
-    </row>
-    <row r="144" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M143" s="4"/>
+      <c r="N143" s="6"/>
+    </row>
+    <row r="144" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="145" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D145" s="4"/>
-      <c r="J145" s="4"/>
       <c r="K145" s="4"/>
       <c r="L145" s="4"/>
-      <c r="M145" s="6"/>
-    </row>
-    <row r="146" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M145" s="4"/>
+      <c r="N145" s="6"/>
+    </row>
+    <row r="146" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D146" s="4"/>
-      <c r="J146" s="4"/>
       <c r="K146" s="4"/>
       <c r="L146" s="4"/>
-      <c r="M146" s="6"/>
-    </row>
-    <row r="147" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M146" s="4"/>
+      <c r="N146" s="6"/>
+    </row>
+    <row r="147" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D147" s="4"/>
-      <c r="J147" s="4"/>
       <c r="K147" s="4"/>
       <c r="L147" s="4"/>
-      <c r="M147" s="6"/>
-    </row>
-    <row r="148" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M147" s="4"/>
+      <c r="N147" s="6"/>
+    </row>
+    <row r="148" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D148" s="4"/>
     </row>
-    <row r="149" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="149" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D149" s="4"/>
       <c r="F149" s="4"/>
-      <c r="J149" s="4"/>
       <c r="K149" s="4"/>
       <c r="L149" s="4"/>
-      <c r="M149" s="6"/>
-    </row>
-    <row r="150" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M149" s="4"/>
+      <c r="N149" s="6"/>
+    </row>
+    <row r="150" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D150" s="4"/>
-      <c r="J150" s="4"/>
       <c r="K150" s="4"/>
       <c r="L150" s="4"/>
-      <c r="M150" s="6"/>
-    </row>
-    <row r="151" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M150" s="4"/>
+      <c r="N150" s="6"/>
+    </row>
+    <row r="151" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D151" s="4"/>
-      <c r="J151" s="4"/>
       <c r="K151" s="4"/>
       <c r="L151" s="4"/>
-      <c r="M151" s="6"/>
-    </row>
-    <row r="152" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M151" s="4"/>
+      <c r="N151" s="6"/>
+    </row>
+    <row r="152" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D152" s="4"/>
-      <c r="J152" s="4"/>
       <c r="K152" s="4"/>
       <c r="L152" s="4"/>
-      <c r="M152" s="6"/>
-    </row>
-    <row r="153" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M152" s="4"/>
+      <c r="N152" s="6"/>
+    </row>
+    <row r="153" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D153" s="4"/>
-      <c r="J153" s="4"/>
       <c r="K153" s="4"/>
       <c r="L153" s="4"/>
-      <c r="M153" s="6"/>
-    </row>
-    <row r="154" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M153" s="4"/>
+      <c r="N153" s="6"/>
+    </row>
+    <row r="154" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D154" s="4"/>
-      <c r="J154" s="4"/>
       <c r="K154" s="4"/>
       <c r="L154" s="4"/>
-      <c r="M154" s="6"/>
-    </row>
-    <row r="155" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M154" s="4"/>
+      <c r="N154" s="6"/>
+    </row>
+    <row r="155" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D155" s="4"/>
-      <c r="J155" s="4"/>
       <c r="K155" s="4"/>
       <c r="L155" s="4"/>
-      <c r="M155" s="6"/>
-    </row>
-    <row r="156" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M155" s="4"/>
+      <c r="N155" s="6"/>
+    </row>
+    <row r="156" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D156" s="4"/>
       <c r="F156" s="4"/>
-      <c r="J156" s="4"/>
       <c r="K156" s="4"/>
       <c r="L156" s="4"/>
-      <c r="M156" s="6"/>
-    </row>
-    <row r="157" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M156" s="4"/>
+      <c r="N156" s="6"/>
+    </row>
+    <row r="157" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D157" s="4"/>
       <c r="F157" s="4"/>
-      <c r="J157" s="4"/>
       <c r="K157" s="4"/>
       <c r="L157" s="4"/>
-      <c r="M157" s="6"/>
-    </row>
-    <row r="158" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M157" s="4"/>
+      <c r="N157" s="6"/>
+    </row>
+    <row r="158" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D158" s="4"/>
-      <c r="J158" s="4"/>
       <c r="K158" s="4"/>
       <c r="L158" s="4"/>
-      <c r="M158" s="6"/>
-    </row>
-    <row r="159" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M158" s="4"/>
+      <c r="N158" s="6"/>
+    </row>
+    <row r="159" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D159" s="4"/>
-      <c r="J159" s="4"/>
       <c r="K159" s="4"/>
       <c r="L159" s="4"/>
-      <c r="M159" s="6"/>
-    </row>
-    <row r="160" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M159" s="4"/>
+      <c r="N159" s="6"/>
+    </row>
+    <row r="160" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D160" s="4"/>
       <c r="F160" s="4"/>
-      <c r="J160" s="4"/>
       <c r="K160" s="4"/>
       <c r="L160" s="4"/>
-      <c r="M160" s="6"/>
-    </row>
-    <row r="161" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M160" s="4"/>
+      <c r="N160" s="6"/>
+    </row>
+    <row r="161" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D161" s="4"/>
       <c r="F161" s="4"/>
-      <c r="J161" s="4"/>
       <c r="K161" s="4"/>
       <c r="L161" s="4"/>
-      <c r="M161" s="6"/>
-    </row>
-    <row r="162" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M161" s="4"/>
+      <c r="N161" s="6"/>
+    </row>
+    <row r="162" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D162" s="4"/>
-      <c r="J162" s="4"/>
       <c r="K162" s="4"/>
       <c r="L162" s="4"/>
-      <c r="M162" s="6"/>
-    </row>
-    <row r="163" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M162" s="4"/>
+      <c r="N162" s="6"/>
+    </row>
+    <row r="163" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D163" s="4"/>
-      <c r="J163" s="4"/>
       <c r="K163" s="4"/>
       <c r="L163" s="4"/>
-      <c r="M163" s="6"/>
-    </row>
-    <row r="164" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M163" s="4"/>
+      <c r="N163" s="6"/>
+    </row>
+    <row r="164" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D164" s="4"/>
       <c r="F164" s="4"/>
-      <c r="J164" s="4"/>
       <c r="K164" s="4"/>
       <c r="L164" s="4"/>
-      <c r="M164" s="6"/>
-    </row>
-    <row r="165" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M164" s="4"/>
+      <c r="N164" s="6"/>
+    </row>
+    <row r="165" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D165" s="4"/>
-      <c r="J165" s="4"/>
       <c r="K165" s="4"/>
       <c r="L165" s="4"/>
-      <c r="M165" s="6"/>
-    </row>
-    <row r="166" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M165" s="4"/>
+      <c r="N165" s="6"/>
+    </row>
+    <row r="166" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D166" s="4"/>
-      <c r="J166" s="4"/>
       <c r="K166" s="4"/>
       <c r="L166" s="4"/>
-      <c r="M166" s="6"/>
-    </row>
-    <row r="167" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M166" s="4"/>
+      <c r="N166" s="6"/>
+    </row>
+    <row r="167" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D167" s="4"/>
-      <c r="J167" s="4"/>
       <c r="K167" s="4"/>
       <c r="L167" s="4"/>
-      <c r="M167" s="6"/>
-    </row>
-    <row r="168" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M167" s="4"/>
+      <c r="N167" s="6"/>
+    </row>
+    <row r="168" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D168" s="4"/>
-      <c r="J168" s="4"/>
       <c r="K168" s="4"/>
       <c r="L168" s="4"/>
-      <c r="M168" s="6"/>
-    </row>
-    <row r="169" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M168" s="4"/>
+      <c r="N168" s="6"/>
+    </row>
+    <row r="169" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D169" s="4"/>
-      <c r="J169" s="4"/>
       <c r="K169" s="4"/>
       <c r="L169" s="4"/>
-      <c r="M169" s="6"/>
-    </row>
-    <row r="170" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M169" s="4"/>
+      <c r="N169" s="6"/>
+    </row>
+    <row r="170" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D170" s="4"/>
-      <c r="J170" s="4"/>
       <c r="K170" s="4"/>
       <c r="L170" s="4"/>
-      <c r="M170" s="6"/>
-    </row>
-    <row r="171" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M170" s="4"/>
+      <c r="N170" s="6"/>
+    </row>
+    <row r="171" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D171" s="4"/>
-      <c r="J171" s="4"/>
       <c r="K171" s="4"/>
       <c r="L171" s="4"/>
-      <c r="M171" s="6"/>
-    </row>
-    <row r="172" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M171" s="4"/>
+      <c r="N171" s="6"/>
+    </row>
+    <row r="172" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D172" s="4"/>
-      <c r="J172" s="4"/>
       <c r="K172" s="4"/>
       <c r="L172" s="4"/>
-      <c r="M172" s="6"/>
-    </row>
-    <row r="173" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M172" s="4"/>
+      <c r="N172" s="6"/>
+    </row>
+    <row r="173" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D173" s="4"/>
-      <c r="J173" s="4"/>
       <c r="K173" s="4"/>
       <c r="L173" s="4"/>
-      <c r="M173" s="6"/>
-    </row>
-    <row r="174" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M173" s="4"/>
+      <c r="N173" s="6"/>
+    </row>
+    <row r="174" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D174" s="4"/>
-      <c r="J174" s="4"/>
       <c r="K174" s="4"/>
       <c r="L174" s="4"/>
-      <c r="M174" s="6"/>
-    </row>
-    <row r="175" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M174" s="4"/>
+      <c r="N174" s="6"/>
+    </row>
+    <row r="175" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D175" s="4"/>
-      <c r="J175" s="4"/>
       <c r="K175" s="4"/>
       <c r="L175" s="4"/>
-      <c r="M175" s="6"/>
-    </row>
-    <row r="176" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M175" s="4"/>
+      <c r="N175" s="6"/>
+    </row>
+    <row r="176" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D176" s="4"/>
       <c r="F176" s="4"/>
-      <c r="J176" s="4"/>
       <c r="K176" s="4"/>
       <c r="L176" s="4"/>
-      <c r="M176" s="6"/>
+      <c r="M176" s="4"/>
+      <c r="N176" s="6"/>
     </row>
     <row r="177" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D177" s="4"/>
@@ -2076,28 +2079,28 @@
   <sheetData>
     <row r="1" spans="1:1024" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>48</v>
       </c>
       <c r="AMG1" s="15"/>
       <c r="AMH1" s="15"/>

</xml_diff>

<commit_message>
fix: code postal dans le fichier de suivi
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AA5D07-3199-0A4E-9D61-85EF3088E633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68627BE1-D668-3249-A40F-4F8D0E885A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23220" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23220" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats Globales" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Date et heure</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Ayants-droits</t>
+  </si>
+  <si>
+    <t>Ville</t>
   </si>
 </sst>
 </file>
@@ -788,11 +791,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMM183"/>
+  <dimension ref="A1:AMN183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -805,17 +808,17 @@
     <col min="6" max="6" width="13.6640625" style="5" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" style="3" customWidth="1"/>
     <col min="8" max="10" width="12.5" style="3" customWidth="1"/>
-    <col min="11" max="12" width="13" style="5" customWidth="1"/>
-    <col min="13" max="13" width="6.1640625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="33" style="3" customWidth="1"/>
-    <col min="15" max="15" width="7.83203125" style="5" customWidth="1"/>
-    <col min="16" max="16" width="35" style="3" customWidth="1"/>
-    <col min="17" max="17" width="44.33203125" style="3" customWidth="1"/>
-    <col min="18" max="1027" width="8.6640625" style="3" customWidth="1"/>
-    <col min="1028" max="16384" width="9.1640625" style="7"/>
+    <col min="11" max="13" width="13" style="5" customWidth="1"/>
+    <col min="14" max="14" width="6.1640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="33" style="3" customWidth="1"/>
+    <col min="16" max="16" width="7.83203125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="35" style="3" customWidth="1"/>
+    <col min="18" max="18" width="44.33203125" style="3" customWidth="1"/>
+    <col min="19" max="1028" width="8.6640625" style="3" customWidth="1"/>
+    <col min="1029" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -853,1180 +856,1330 @@
         <v>34</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D2" s="4"/>
       <c r="F2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N2" s="4"/>
+      <c r="O2" s="6"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="6"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N3" s="4"/>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N4" s="4"/>
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="6"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N5" s="4"/>
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="6"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N6" s="4"/>
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="6"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N7" s="4"/>
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N8" s="4"/>
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="6"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N9" s="4"/>
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="6"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N10" s="4"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N11" s="4"/>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="6"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N12" s="4"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="6"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N13" s="4"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N14" s="4"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-      <c r="N15" s="6"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N15" s="4"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="N17" s="6"/>
-    </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N17" s="4"/>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
-      <c r="N18" s="6"/>
-    </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N18" s="4"/>
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="6"/>
-    </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N19" s="4"/>
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="6"/>
-    </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N20" s="4"/>
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="6"/>
-    </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N21" s="4"/>
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
-      <c r="N22" s="6"/>
-    </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N22" s="4"/>
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
-      <c r="N23" s="6"/>
-    </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N23" s="4"/>
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="6"/>
-    </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N24" s="4"/>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="26" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D26" s="4"/>
       <c r="F26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
-      <c r="N26" s="6"/>
-    </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N26" s="4"/>
+      <c r="O26" s="6"/>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
-      <c r="N27" s="6"/>
-    </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N27" s="4"/>
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
-      <c r="N28" s="6"/>
-    </row>
-    <row r="29" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N28" s="4"/>
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
-      <c r="N29" s="6"/>
-    </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N29" s="4"/>
+      <c r="O29" s="6"/>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
-      <c r="N30" s="6"/>
-    </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N30" s="4"/>
+      <c r="O30" s="6"/>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
-      <c r="N31" s="6"/>
-    </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N31" s="4"/>
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
-      <c r="N32" s="6"/>
-    </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N32" s="4"/>
+      <c r="O32" s="6"/>
+    </row>
+    <row r="33" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
-      <c r="N33" s="6"/>
-    </row>
-    <row r="34" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N33" s="4"/>
+      <c r="O33" s="6"/>
+    </row>
+    <row r="34" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
-      <c r="N34" s="6"/>
-    </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N34" s="4"/>
+      <c r="O34" s="6"/>
+    </row>
+    <row r="35" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="36" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="37" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
-      <c r="N37" s="6"/>
-    </row>
-    <row r="38" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N37" s="4"/>
+      <c r="O37" s="6"/>
+    </row>
+    <row r="38" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="39" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
-      <c r="N39" s="6"/>
-    </row>
-    <row r="40" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N39" s="4"/>
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
-      <c r="N40" s="6"/>
-    </row>
-    <row r="41" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N40" s="4"/>
+      <c r="O40" s="6"/>
+    </row>
+    <row r="41" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
-      <c r="N41" s="6"/>
-    </row>
-    <row r="42" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N41" s="4"/>
+      <c r="O41" s="6"/>
+    </row>
+    <row r="42" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D42" s="4"/>
       <c r="F42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
-      <c r="N42" s="6"/>
-    </row>
-    <row r="43" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N42" s="4"/>
+      <c r="O42" s="6"/>
+    </row>
+    <row r="43" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
-      <c r="N43" s="6"/>
-    </row>
-    <row r="44" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N43" s="4"/>
+      <c r="O43" s="6"/>
+    </row>
+    <row r="44" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D44" s="4"/>
       <c r="F44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
-      <c r="N44" s="6"/>
-    </row>
-    <row r="45" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N44" s="4"/>
+      <c r="O44" s="6"/>
+    </row>
+    <row r="45" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
-      <c r="N45" s="6"/>
-    </row>
-    <row r="46" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N45" s="4"/>
+      <c r="O45" s="6"/>
+    </row>
+    <row r="46" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="47" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="48" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="49" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
-      <c r="N49" s="6"/>
-    </row>
-    <row r="50" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N49" s="4"/>
+      <c r="O49" s="6"/>
+    </row>
+    <row r="50" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="51" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="52" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
-      <c r="N52" s="6"/>
-    </row>
-    <row r="53" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N52" s="4"/>
+      <c r="O52" s="6"/>
+    </row>
+    <row r="53" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D53" s="4"/>
       <c r="F53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
-      <c r="N53" s="6"/>
-    </row>
-    <row r="54" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N53" s="4"/>
+      <c r="O53" s="6"/>
+    </row>
+    <row r="54" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="55" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="56" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="57" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D57" s="4"/>
       <c r="F57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
-      <c r="N57" s="6"/>
-    </row>
-    <row r="58" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N57" s="4"/>
+      <c r="O57" s="6"/>
+    </row>
+    <row r="58" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D58" s="4"/>
       <c r="F58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
-      <c r="N58" s="6"/>
-    </row>
-    <row r="59" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N58" s="4"/>
+      <c r="O58" s="6"/>
+    </row>
+    <row r="59" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="60" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D60" s="4"/>
       <c r="F60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
-      <c r="N60" s="6"/>
-    </row>
-    <row r="61" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N60" s="4"/>
+      <c r="O60" s="6"/>
+    </row>
+    <row r="61" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
-      <c r="N61" s="6"/>
-    </row>
-    <row r="62" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N61" s="4"/>
+      <c r="O61" s="6"/>
+    </row>
+    <row r="62" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
-      <c r="N62" s="6"/>
-    </row>
-    <row r="63" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N62" s="4"/>
+      <c r="O62" s="6"/>
+    </row>
+    <row r="63" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="64" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D64" s="4"/>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
-      <c r="N64" s="6"/>
-    </row>
-    <row r="65" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N64" s="4"/>
+      <c r="O64" s="6"/>
+    </row>
+    <row r="65" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="66" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D66" s="4"/>
       <c r="F66" s="4"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
-      <c r="N66" s="6"/>
-    </row>
-    <row r="67" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N66" s="4"/>
+      <c r="O66" s="6"/>
+    </row>
+    <row r="67" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
-      <c r="N67" s="6"/>
-    </row>
-    <row r="68" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N67" s="4"/>
+      <c r="O67" s="6"/>
+    </row>
+    <row r="68" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D68" s="4"/>
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
-      <c r="N68" s="6"/>
-    </row>
-    <row r="69" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N68" s="4"/>
+      <c r="O68" s="6"/>
+    </row>
+    <row r="69" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
-      <c r="N69" s="6"/>
-    </row>
-    <row r="70" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N69" s="4"/>
+      <c r="O69" s="6"/>
+    </row>
+    <row r="70" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
-      <c r="N70" s="6"/>
-    </row>
-    <row r="71" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N70" s="4"/>
+      <c r="O70" s="6"/>
+    </row>
+    <row r="71" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D71" s="4"/>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
-      <c r="N71" s="6"/>
-    </row>
-    <row r="72" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N71" s="4"/>
+      <c r="O71" s="6"/>
+    </row>
+    <row r="72" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D72" s="4"/>
       <c r="F72" s="4"/>
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
-      <c r="N72" s="6"/>
-    </row>
-    <row r="73" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N72" s="4"/>
+      <c r="O72" s="6"/>
+    </row>
+    <row r="73" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="74" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D74" s="4"/>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
-      <c r="N74" s="6"/>
-    </row>
-    <row r="75" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N74" s="4"/>
+      <c r="O74" s="6"/>
+    </row>
+    <row r="75" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D75" s="4"/>
       <c r="F75" s="4"/>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
-      <c r="N75" s="6"/>
-    </row>
-    <row r="76" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N75" s="4"/>
+      <c r="O75" s="6"/>
+    </row>
+    <row r="76" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="77" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D77" s="4"/>
       <c r="F77" s="4"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
-      <c r="N77" s="6"/>
-    </row>
-    <row r="78" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N77" s="4"/>
+      <c r="O77" s="6"/>
+    </row>
+    <row r="78" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="79" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D79" s="4"/>
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
       <c r="M79" s="4"/>
-      <c r="N79" s="6"/>
-    </row>
-    <row r="80" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N79" s="4"/>
+      <c r="O79" s="6"/>
+    </row>
+    <row r="80" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D80" s="4"/>
     </row>
-    <row r="81" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="81" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D81" s="4"/>
       <c r="F81" s="4"/>
       <c r="K81" s="4"/>
       <c r="L81" s="4"/>
       <c r="M81" s="4"/>
-      <c r="N81" s="6"/>
-    </row>
-    <row r="82" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N81" s="4"/>
+      <c r="O81" s="6"/>
+    </row>
+    <row r="82" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D82" s="4"/>
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
       <c r="M82" s="4"/>
-      <c r="N82" s="6"/>
-    </row>
-    <row r="83" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N82" s="4"/>
+      <c r="O82" s="6"/>
+    </row>
+    <row r="83" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="84" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D84" s="4"/>
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
       <c r="M84" s="4"/>
-      <c r="N84" s="6"/>
-    </row>
-    <row r="85" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N84" s="4"/>
+      <c r="O84" s="6"/>
+    </row>
+    <row r="85" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D85" s="4"/>
       <c r="F85" s="4"/>
       <c r="K85" s="4"/>
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
-      <c r="N85" s="6"/>
-    </row>
-    <row r="86" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N85" s="4"/>
+      <c r="O85" s="6"/>
+    </row>
+    <row r="86" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D86" s="4"/>
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
-      <c r="N86" s="6"/>
-    </row>
-    <row r="87" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N86" s="4"/>
+      <c r="O86" s="6"/>
+    </row>
+    <row r="87" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="88" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D88" s="4"/>
       <c r="F88" s="4"/>
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
-      <c r="N88" s="6"/>
-    </row>
-    <row r="89" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N88" s="4"/>
+      <c r="O88" s="6"/>
+    </row>
+    <row r="89" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D89" s="4"/>
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
       <c r="M89" s="4"/>
-      <c r="N89" s="6"/>
-    </row>
-    <row r="90" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N89" s="4"/>
+      <c r="O89" s="6"/>
+    </row>
+    <row r="90" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D90" s="4"/>
       <c r="F90" s="4"/>
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
       <c r="M90" s="4"/>
-      <c r="N90" s="6"/>
-    </row>
-    <row r="91" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N90" s="4"/>
+      <c r="O90" s="6"/>
+    </row>
+    <row r="91" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D91" s="4"/>
       <c r="F91" s="4"/>
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
       <c r="M91" s="4"/>
-      <c r="N91" s="6"/>
-    </row>
-    <row r="92" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N91" s="4"/>
+      <c r="O91" s="6"/>
+    </row>
+    <row r="92" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D92" s="4"/>
       <c r="F92" s="4"/>
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
-      <c r="N92" s="6"/>
-    </row>
-    <row r="93" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N92" s="4"/>
+      <c r="O92" s="6"/>
+    </row>
+    <row r="93" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D93" s="4"/>
       <c r="F93" s="4"/>
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
-      <c r="N93" s="6"/>
-    </row>
-    <row r="94" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N93" s="4"/>
+      <c r="O93" s="6"/>
+    </row>
+    <row r="94" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D94" s="4"/>
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
       <c r="M94" s="4"/>
-      <c r="N94" s="6"/>
-    </row>
-    <row r="95" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N94" s="4"/>
+      <c r="O94" s="6"/>
+    </row>
+    <row r="95" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D95" s="4"/>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
-      <c r="N95" s="6"/>
-    </row>
-    <row r="96" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N95" s="4"/>
+      <c r="O95" s="6"/>
+    </row>
+    <row r="96" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D96" s="4"/>
       <c r="K96" s="4"/>
       <c r="L96" s="4"/>
       <c r="M96" s="4"/>
-      <c r="N96" s="6"/>
-    </row>
-    <row r="97" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N96" s="4"/>
+      <c r="O96" s="6"/>
+    </row>
+    <row r="97" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D97" s="4"/>
       <c r="F97" s="4"/>
       <c r="K97" s="4"/>
       <c r="L97" s="4"/>
       <c r="M97" s="4"/>
-      <c r="N97" s="6"/>
-    </row>
-    <row r="98" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N97" s="4"/>
+      <c r="O97" s="6"/>
+    </row>
+    <row r="98" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D98" s="4"/>
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
-      <c r="N98" s="6"/>
-    </row>
-    <row r="99" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N98" s="4"/>
+      <c r="O98" s="6"/>
+    </row>
+    <row r="99" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D99" s="4"/>
       <c r="F99" s="4"/>
       <c r="K99" s="4"/>
       <c r="L99" s="4"/>
       <c r="M99" s="4"/>
-      <c r="N99" s="6"/>
-    </row>
-    <row r="100" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N99" s="4"/>
+      <c r="O99" s="6"/>
+    </row>
+    <row r="100" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D100" s="4"/>
       <c r="F100" s="4"/>
       <c r="K100" s="4"/>
       <c r="L100" s="4"/>
       <c r="M100" s="4"/>
-      <c r="N100" s="6"/>
-    </row>
-    <row r="101" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N100" s="4"/>
+      <c r="O100" s="6"/>
+    </row>
+    <row r="101" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D101" s="4"/>
       <c r="F101" s="4"/>
       <c r="K101" s="4"/>
       <c r="L101" s="4"/>
       <c r="M101" s="4"/>
-      <c r="N101" s="6"/>
-    </row>
-    <row r="102" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N101" s="4"/>
+      <c r="O101" s="6"/>
+    </row>
+    <row r="102" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D102" s="4"/>
       <c r="F102" s="4"/>
       <c r="K102" s="4"/>
       <c r="L102" s="4"/>
       <c r="M102" s="4"/>
-      <c r="N102" s="6"/>
-    </row>
-    <row r="103" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N102" s="4"/>
+      <c r="O102" s="6"/>
+    </row>
+    <row r="103" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D103" s="4"/>
       <c r="K103" s="4"/>
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
-      <c r="N103" s="6"/>
-    </row>
-    <row r="104" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N103" s="4"/>
+      <c r="O103" s="6"/>
+    </row>
+    <row r="104" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D104" s="4"/>
       <c r="K104" s="4"/>
       <c r="L104" s="4"/>
       <c r="M104" s="4"/>
-      <c r="N104" s="6"/>
-    </row>
-    <row r="105" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N104" s="4"/>
+      <c r="O104" s="6"/>
+    </row>
+    <row r="105" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D105" s="4"/>
       <c r="F105" s="4"/>
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
       <c r="M105" s="4"/>
-      <c r="N105" s="6"/>
-    </row>
-    <row r="106" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N105" s="4"/>
+      <c r="O105" s="6"/>
+    </row>
+    <row r="106" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D106" s="4"/>
       <c r="F106" s="4"/>
       <c r="K106" s="4"/>
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
-      <c r="N106" s="6"/>
-    </row>
-    <row r="107" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N106" s="4"/>
+      <c r="O106" s="6"/>
+    </row>
+    <row r="107" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D107" s="4"/>
       <c r="K107" s="4"/>
       <c r="L107" s="4"/>
       <c r="M107" s="4"/>
-      <c r="N107" s="6"/>
-    </row>
-    <row r="108" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N107" s="4"/>
+      <c r="O107" s="6"/>
+    </row>
+    <row r="108" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D108" s="4"/>
       <c r="F108" s="4"/>
       <c r="K108" s="4"/>
       <c r="L108" s="4"/>
       <c r="M108" s="4"/>
-      <c r="N108" s="6"/>
-    </row>
-    <row r="109" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N108" s="4"/>
+      <c r="O108" s="6"/>
+    </row>
+    <row r="109" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D109" s="4"/>
       <c r="F109" s="4"/>
       <c r="K109" s="4"/>
       <c r="L109" s="4"/>
       <c r="M109" s="4"/>
-      <c r="N109" s="6"/>
-    </row>
-    <row r="110" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N109" s="4"/>
+      <c r="O109" s="6"/>
+    </row>
+    <row r="110" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D110" s="4"/>
       <c r="K110" s="4"/>
       <c r="L110" s="4"/>
       <c r="M110" s="4"/>
-      <c r="N110" s="6"/>
-    </row>
-    <row r="111" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N110" s="4"/>
+      <c r="O110" s="6"/>
+    </row>
+    <row r="111" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D111" s="4"/>
       <c r="F111" s="4"/>
       <c r="K111" s="4"/>
       <c r="L111" s="4"/>
       <c r="M111" s="4"/>
-      <c r="N111" s="6"/>
-    </row>
-    <row r="112" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N111" s="4"/>
+      <c r="O111" s="6"/>
+    </row>
+    <row r="112" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D112" s="4"/>
       <c r="K112" s="4"/>
       <c r="L112" s="4"/>
       <c r="M112" s="4"/>
-      <c r="N112" s="6"/>
-    </row>
-    <row r="113" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N112" s="4"/>
+      <c r="O112" s="6"/>
+    </row>
+    <row r="113" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D113" s="4"/>
       <c r="K113" s="4"/>
       <c r="L113" s="4"/>
       <c r="M113" s="4"/>
-      <c r="N113" s="6"/>
-    </row>
-    <row r="114" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N113" s="4"/>
+      <c r="O113" s="6"/>
+    </row>
+    <row r="114" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D114" s="4"/>
       <c r="K114" s="4"/>
       <c r="L114" s="4"/>
       <c r="M114" s="4"/>
-      <c r="N114" s="6"/>
-    </row>
-    <row r="115" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N114" s="4"/>
+      <c r="O114" s="6"/>
+    </row>
+    <row r="115" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D115" s="4"/>
       <c r="F115" s="4"/>
       <c r="K115" s="4"/>
       <c r="L115" s="4"/>
       <c r="M115" s="4"/>
-      <c r="N115" s="6"/>
-    </row>
-    <row r="116" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N115" s="4"/>
+      <c r="O115" s="6"/>
+    </row>
+    <row r="116" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D116" s="4"/>
       <c r="F116" s="4"/>
       <c r="K116" s="4"/>
       <c r="L116" s="4"/>
       <c r="M116" s="4"/>
-      <c r="N116" s="6"/>
-    </row>
-    <row r="117" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N116" s="4"/>
+      <c r="O116" s="6"/>
+    </row>
+    <row r="117" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D117" s="4"/>
       <c r="F117" s="4"/>
       <c r="K117" s="4"/>
       <c r="L117" s="4"/>
       <c r="M117" s="4"/>
-      <c r="N117" s="6"/>
-    </row>
-    <row r="118" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N117" s="4"/>
+      <c r="O117" s="6"/>
+    </row>
+    <row r="118" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D118" s="4"/>
       <c r="F118" s="4"/>
       <c r="K118" s="4"/>
       <c r="L118" s="4"/>
       <c r="M118" s="4"/>
-      <c r="N118" s="6"/>
-    </row>
-    <row r="119" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N118" s="4"/>
+      <c r="O118" s="6"/>
+    </row>
+    <row r="119" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D119" s="4"/>
       <c r="F119" s="4"/>
       <c r="K119" s="4"/>
       <c r="L119" s="4"/>
       <c r="M119" s="4"/>
-      <c r="N119" s="6"/>
-    </row>
-    <row r="120" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N119" s="4"/>
+      <c r="O119" s="6"/>
+    </row>
+    <row r="120" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D120" s="4"/>
       <c r="F120" s="4"/>
       <c r="K120" s="4"/>
       <c r="L120" s="4"/>
       <c r="M120" s="4"/>
-      <c r="N120" s="6"/>
-    </row>
-    <row r="121" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N120" s="4"/>
+      <c r="O120" s="6"/>
+    </row>
+    <row r="121" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D121" s="4"/>
       <c r="K121" s="4"/>
       <c r="L121" s="4"/>
       <c r="M121" s="4"/>
-      <c r="N121" s="6"/>
-    </row>
-    <row r="122" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N121" s="4"/>
+      <c r="O121" s="6"/>
+    </row>
+    <row r="122" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D122" s="4"/>
       <c r="K122" s="4"/>
       <c r="L122" s="4"/>
       <c r="M122" s="4"/>
-      <c r="N122" s="6"/>
-    </row>
-    <row r="123" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N122" s="4"/>
+      <c r="O122" s="6"/>
+    </row>
+    <row r="123" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D123" s="4"/>
       <c r="K123" s="4"/>
       <c r="L123" s="4"/>
       <c r="M123" s="4"/>
-      <c r="N123" s="6"/>
-    </row>
-    <row r="124" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N123" s="4"/>
+      <c r="O123" s="6"/>
+    </row>
+    <row r="124" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D124" s="4"/>
       <c r="K124" s="4"/>
       <c r="L124" s="4"/>
       <c r="M124" s="4"/>
-      <c r="N124" s="6"/>
-    </row>
-    <row r="125" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N124" s="4"/>
+      <c r="O124" s="6"/>
+    </row>
+    <row r="125" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D125" s="4"/>
       <c r="K125" s="4"/>
       <c r="L125" s="4"/>
       <c r="M125" s="4"/>
-      <c r="N125" s="6"/>
-    </row>
-    <row r="126" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N125" s="4"/>
+      <c r="O125" s="6"/>
+    </row>
+    <row r="126" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D126" s="4"/>
       <c r="F126" s="4"/>
       <c r="K126" s="4"/>
       <c r="L126" s="4"/>
       <c r="M126" s="4"/>
-      <c r="N126" s="6"/>
-    </row>
-    <row r="127" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N126" s="4"/>
+      <c r="O126" s="6"/>
+    </row>
+    <row r="127" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D127" s="4"/>
       <c r="K127" s="4"/>
       <c r="L127" s="4"/>
       <c r="M127" s="4"/>
-      <c r="N127" s="6"/>
-    </row>
-    <row r="128" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N127" s="4"/>
+      <c r="O127" s="6"/>
+    </row>
+    <row r="128" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D128" s="4"/>
       <c r="K128" s="4"/>
       <c r="L128" s="4"/>
       <c r="M128" s="4"/>
-      <c r="N128" s="6"/>
-    </row>
-    <row r="129" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N128" s="4"/>
+      <c r="O128" s="6"/>
+    </row>
+    <row r="129" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="130" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D130" s="4"/>
       <c r="K130" s="4"/>
       <c r="L130" s="4"/>
       <c r="M130" s="4"/>
-      <c r="N130" s="6"/>
-    </row>
-    <row r="131" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N130" s="4"/>
+      <c r="O130" s="6"/>
+    </row>
+    <row r="131" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="132" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D132" s="4"/>
       <c r="F132" s="4"/>
       <c r="K132" s="4"/>
       <c r="L132" s="4"/>
       <c r="M132" s="4"/>
-      <c r="N132" s="6"/>
-    </row>
-    <row r="133" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N132" s="4"/>
+      <c r="O132" s="6"/>
+    </row>
+    <row r="133" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D133" s="4"/>
       <c r="K133" s="4"/>
       <c r="L133" s="4"/>
       <c r="M133" s="4"/>
-      <c r="N133" s="6"/>
-    </row>
-    <row r="134" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N133" s="4"/>
+      <c r="O133" s="6"/>
+    </row>
+    <row r="134" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D134" s="4"/>
       <c r="K134" s="4"/>
       <c r="L134" s="4"/>
       <c r="M134" s="4"/>
-      <c r="N134" s="6"/>
-    </row>
-    <row r="135" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N134" s="4"/>
+      <c r="O134" s="6"/>
+    </row>
+    <row r="135" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D135" s="4"/>
       <c r="K135" s="4"/>
       <c r="L135" s="4"/>
       <c r="M135" s="4"/>
-      <c r="N135" s="6"/>
-    </row>
-    <row r="136" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N135" s="4"/>
+      <c r="O135" s="6"/>
+    </row>
+    <row r="136" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D136" s="4"/>
       <c r="K136" s="4"/>
       <c r="L136" s="4"/>
       <c r="M136" s="4"/>
-      <c r="N136" s="6"/>
-    </row>
-    <row r="137" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N136" s="4"/>
+      <c r="O136" s="6"/>
+    </row>
+    <row r="137" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="138" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="139" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D139" s="4"/>
       <c r="K139" s="4"/>
       <c r="L139" s="4"/>
       <c r="M139" s="4"/>
-      <c r="N139" s="6"/>
-    </row>
-    <row r="140" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N139" s="4"/>
+      <c r="O139" s="6"/>
+    </row>
+    <row r="140" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D140" s="4"/>
       <c r="K140" s="4"/>
       <c r="L140" s="4"/>
       <c r="M140" s="4"/>
-      <c r="N140" s="6"/>
-    </row>
-    <row r="141" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N140" s="4"/>
+      <c r="O140" s="6"/>
+    </row>
+    <row r="141" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D141" s="4"/>
       <c r="K141" s="4"/>
       <c r="L141" s="4"/>
       <c r="M141" s="4"/>
-      <c r="N141" s="6"/>
-    </row>
-    <row r="142" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N141" s="4"/>
+      <c r="O141" s="6"/>
+    </row>
+    <row r="142" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D142" s="4"/>
       <c r="K142" s="4"/>
       <c r="L142" s="4"/>
       <c r="M142" s="4"/>
-      <c r="N142" s="6"/>
-    </row>
-    <row r="143" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N142" s="4"/>
+      <c r="O142" s="6"/>
+    </row>
+    <row r="143" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D143" s="4"/>
       <c r="K143" s="4"/>
       <c r="L143" s="4"/>
       <c r="M143" s="4"/>
-      <c r="N143" s="6"/>
-    </row>
-    <row r="144" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N143" s="4"/>
+      <c r="O143" s="6"/>
+    </row>
+    <row r="144" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="145" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D145" s="4"/>
       <c r="K145" s="4"/>
       <c r="L145" s="4"/>
       <c r="M145" s="4"/>
-      <c r="N145" s="6"/>
-    </row>
-    <row r="146" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N145" s="4"/>
+      <c r="O145" s="6"/>
+    </row>
+    <row r="146" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D146" s="4"/>
       <c r="K146" s="4"/>
       <c r="L146" s="4"/>
       <c r="M146" s="4"/>
-      <c r="N146" s="6"/>
-    </row>
-    <row r="147" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N146" s="4"/>
+      <c r="O146" s="6"/>
+    </row>
+    <row r="147" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D147" s="4"/>
       <c r="K147" s="4"/>
       <c r="L147" s="4"/>
       <c r="M147" s="4"/>
-      <c r="N147" s="6"/>
-    </row>
-    <row r="148" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N147" s="4"/>
+      <c r="O147" s="6"/>
+    </row>
+    <row r="148" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D148" s="4"/>
     </row>
-    <row r="149" spans="4:14" x14ac:dyDescent="0.15">
+    <row r="149" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D149" s="4"/>
       <c r="F149" s="4"/>
       <c r="K149" s="4"/>
       <c r="L149" s="4"/>
       <c r="M149" s="4"/>
-      <c r="N149" s="6"/>
-    </row>
-    <row r="150" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N149" s="4"/>
+      <c r="O149" s="6"/>
+    </row>
+    <row r="150" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D150" s="4"/>
       <c r="K150" s="4"/>
       <c r="L150" s="4"/>
       <c r="M150" s="4"/>
-      <c r="N150" s="6"/>
-    </row>
-    <row r="151" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N150" s="4"/>
+      <c r="O150" s="6"/>
+    </row>
+    <row r="151" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D151" s="4"/>
       <c r="K151" s="4"/>
       <c r="L151" s="4"/>
       <c r="M151" s="4"/>
-      <c r="N151" s="6"/>
-    </row>
-    <row r="152" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N151" s="4"/>
+      <c r="O151" s="6"/>
+    </row>
+    <row r="152" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D152" s="4"/>
       <c r="K152" s="4"/>
       <c r="L152" s="4"/>
       <c r="M152" s="4"/>
-      <c r="N152" s="6"/>
-    </row>
-    <row r="153" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N152" s="4"/>
+      <c r="O152" s="6"/>
+    </row>
+    <row r="153" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D153" s="4"/>
       <c r="K153" s="4"/>
       <c r="L153" s="4"/>
       <c r="M153" s="4"/>
-      <c r="N153" s="6"/>
-    </row>
-    <row r="154" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N153" s="4"/>
+      <c r="O153" s="6"/>
+    </row>
+    <row r="154" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D154" s="4"/>
       <c r="K154" s="4"/>
       <c r="L154" s="4"/>
       <c r="M154" s="4"/>
-      <c r="N154" s="6"/>
-    </row>
-    <row r="155" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N154" s="4"/>
+      <c r="O154" s="6"/>
+    </row>
+    <row r="155" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D155" s="4"/>
       <c r="K155" s="4"/>
       <c r="L155" s="4"/>
       <c r="M155" s="4"/>
-      <c r="N155" s="6"/>
-    </row>
-    <row r="156" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N155" s="4"/>
+      <c r="O155" s="6"/>
+    </row>
+    <row r="156" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D156" s="4"/>
       <c r="F156" s="4"/>
       <c r="K156" s="4"/>
       <c r="L156" s="4"/>
       <c r="M156" s="4"/>
-      <c r="N156" s="6"/>
-    </row>
-    <row r="157" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N156" s="4"/>
+      <c r="O156" s="6"/>
+    </row>
+    <row r="157" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D157" s="4"/>
       <c r="F157" s="4"/>
       <c r="K157" s="4"/>
       <c r="L157" s="4"/>
       <c r="M157" s="4"/>
-      <c r="N157" s="6"/>
-    </row>
-    <row r="158" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N157" s="4"/>
+      <c r="O157" s="6"/>
+    </row>
+    <row r="158" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D158" s="4"/>
       <c r="K158" s="4"/>
       <c r="L158" s="4"/>
       <c r="M158" s="4"/>
-      <c r="N158" s="6"/>
-    </row>
-    <row r="159" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N158" s="4"/>
+      <c r="O158" s="6"/>
+    </row>
+    <row r="159" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D159" s="4"/>
       <c r="K159" s="4"/>
       <c r="L159" s="4"/>
       <c r="M159" s="4"/>
-      <c r="N159" s="6"/>
-    </row>
-    <row r="160" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N159" s="4"/>
+      <c r="O159" s="6"/>
+    </row>
+    <row r="160" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D160" s="4"/>
       <c r="F160" s="4"/>
       <c r="K160" s="4"/>
       <c r="L160" s="4"/>
       <c r="M160" s="4"/>
-      <c r="N160" s="6"/>
-    </row>
-    <row r="161" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N160" s="4"/>
+      <c r="O160" s="6"/>
+    </row>
+    <row r="161" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D161" s="4"/>
       <c r="F161" s="4"/>
       <c r="K161" s="4"/>
       <c r="L161" s="4"/>
       <c r="M161" s="4"/>
-      <c r="N161" s="6"/>
-    </row>
-    <row r="162" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N161" s="4"/>
+      <c r="O161" s="6"/>
+    </row>
+    <row r="162" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D162" s="4"/>
       <c r="K162" s="4"/>
       <c r="L162" s="4"/>
       <c r="M162" s="4"/>
-      <c r="N162" s="6"/>
-    </row>
-    <row r="163" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N162" s="4"/>
+      <c r="O162" s="6"/>
+    </row>
+    <row r="163" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D163" s="4"/>
       <c r="K163" s="4"/>
       <c r="L163" s="4"/>
       <c r="M163" s="4"/>
-      <c r="N163" s="6"/>
-    </row>
-    <row r="164" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N163" s="4"/>
+      <c r="O163" s="6"/>
+    </row>
+    <row r="164" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D164" s="4"/>
       <c r="F164" s="4"/>
       <c r="K164" s="4"/>
       <c r="L164" s="4"/>
       <c r="M164" s="4"/>
-      <c r="N164" s="6"/>
-    </row>
-    <row r="165" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N164" s="4"/>
+      <c r="O164" s="6"/>
+    </row>
+    <row r="165" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D165" s="4"/>
       <c r="K165" s="4"/>
       <c r="L165" s="4"/>
       <c r="M165" s="4"/>
-      <c r="N165" s="6"/>
-    </row>
-    <row r="166" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N165" s="4"/>
+      <c r="O165" s="6"/>
+    </row>
+    <row r="166" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D166" s="4"/>
       <c r="K166" s="4"/>
       <c r="L166" s="4"/>
       <c r="M166" s="4"/>
-      <c r="N166" s="6"/>
-    </row>
-    <row r="167" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N166" s="4"/>
+      <c r="O166" s="6"/>
+    </row>
+    <row r="167" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D167" s="4"/>
       <c r="K167" s="4"/>
       <c r="L167" s="4"/>
       <c r="M167" s="4"/>
-      <c r="N167" s="6"/>
-    </row>
-    <row r="168" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N167" s="4"/>
+      <c r="O167" s="6"/>
+    </row>
+    <row r="168" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D168" s="4"/>
       <c r="K168" s="4"/>
       <c r="L168" s="4"/>
       <c r="M168" s="4"/>
-      <c r="N168" s="6"/>
-    </row>
-    <row r="169" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N168" s="4"/>
+      <c r="O168" s="6"/>
+    </row>
+    <row r="169" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D169" s="4"/>
       <c r="K169" s="4"/>
       <c r="L169" s="4"/>
       <c r="M169" s="4"/>
-      <c r="N169" s="6"/>
-    </row>
-    <row r="170" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N169" s="4"/>
+      <c r="O169" s="6"/>
+    </row>
+    <row r="170" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D170" s="4"/>
       <c r="K170" s="4"/>
       <c r="L170" s="4"/>
       <c r="M170" s="4"/>
-      <c r="N170" s="6"/>
-    </row>
-    <row r="171" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N170" s="4"/>
+      <c r="O170" s="6"/>
+    </row>
+    <row r="171" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D171" s="4"/>
       <c r="K171" s="4"/>
       <c r="L171" s="4"/>
       <c r="M171" s="4"/>
-      <c r="N171" s="6"/>
-    </row>
-    <row r="172" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N171" s="4"/>
+      <c r="O171" s="6"/>
+    </row>
+    <row r="172" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D172" s="4"/>
       <c r="K172" s="4"/>
       <c r="L172" s="4"/>
       <c r="M172" s="4"/>
-      <c r="N172" s="6"/>
-    </row>
-    <row r="173" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N172" s="4"/>
+      <c r="O172" s="6"/>
+    </row>
+    <row r="173" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D173" s="4"/>
       <c r="K173" s="4"/>
       <c r="L173" s="4"/>
       <c r="M173" s="4"/>
-      <c r="N173" s="6"/>
-    </row>
-    <row r="174" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N173" s="4"/>
+      <c r="O173" s="6"/>
+    </row>
+    <row r="174" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D174" s="4"/>
       <c r="K174" s="4"/>
       <c r="L174" s="4"/>
       <c r="M174" s="4"/>
-      <c r="N174" s="6"/>
-    </row>
-    <row r="175" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N174" s="4"/>
+      <c r="O174" s="6"/>
+    </row>
+    <row r="175" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D175" s="4"/>
       <c r="K175" s="4"/>
       <c r="L175" s="4"/>
       <c r="M175" s="4"/>
-      <c r="N175" s="6"/>
-    </row>
-    <row r="176" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="N175" s="4"/>
+      <c r="O175" s="6"/>
+    </row>
+    <row r="176" spans="4:15" x14ac:dyDescent="0.15">
       <c r="D176" s="4"/>
       <c r="F176" s="4"/>
       <c r="K176" s="4"/>
       <c r="L176" s="4"/>
       <c r="M176" s="4"/>
-      <c r="N176" s="6"/>
+      <c r="N176" s="4"/>
+      <c r="O176" s="6"/>
     </row>
     <row r="177" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D177" s="4"/>

</xml_diff>

<commit_message>
fix(stats): ajout de la nouvelle donnée de connexion au portail dans les stats
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68627BE1-D668-3249-A40F-4F8D0E885A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA1DF1C-FE3B-4146-9618-4FB2C05185E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23220" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23220" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats Globales" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>Date et heure</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Documents uploadés</t>
-  </si>
-  <si>
-    <t>Intéractions</t>
   </si>
   <si>
     <t>Appels téléphoniques</t>
@@ -187,6 +184,12 @@
   </si>
   <si>
     <t>Ville</t>
+  </si>
+  <si>
+    <t>Connexions au portail</t>
+  </si>
+  <si>
+    <t>Interactions</t>
   </si>
 </sst>
 </file>
@@ -574,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -609,7 +612,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="9"/>
       <c r="D4" s="9"/>
@@ -726,62 +729,67 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="9"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="9"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="12"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="9"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -793,7 +801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMN183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
     </sheetView>
@@ -820,58 +828,58 @@
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
@@ -2232,28 +2240,28 @@
   <sheetData>
     <row r="1" spans="1:1024" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>47</v>
       </c>
       <c r="AMG1" s="15"/>
       <c r="AMH1" s="15"/>

</xml_diff>

<commit_message>
fix(stats): correction de la stats sur le portail
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA1DF1C-FE3B-4146-9618-4FB2C05185E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55687510-6C36-484B-9C2B-C9C86AAB8E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="23220" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
fix(labels): harmonisation du terme portail usager
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55687510-6C36-484B-9C2B-C9C86AAB8E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512CD788-CB8C-6D4A-9463-4CECC94F5849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23220" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats Globales" sheetId="1" r:id="rId1"/>
@@ -186,10 +186,10 @@
     <t>Ville</t>
   </si>
   <si>
-    <t>Connexions au portail</t>
-  </si>
-  <si>
     <t>Interactions</t>
+  </si>
+  <si>
+    <t>Connexions au portail usager</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -788,7 +788,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(notes): affichage des notes dans le formulaire fix(excel): ajout du total des passages dans les exports
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512CD788-CB8C-6D4A-9463-4CECC94F5849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D80144-1412-944D-BF05-7232A4947CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Date et heure</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Connexions au portail usager</t>
+  </si>
+  <si>
+    <t>Passages avec remise de courrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passages sans remise de courrier	</t>
   </si>
 </sst>
 </file>
@@ -252,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
@@ -296,6 +302,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -780,14 +789,24 @@
       </c>
       <c r="B29" s="9"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="9" t="s">
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="9"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="7" t="s">
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="7" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(docker): mise à jour de nginx4spa fix(rgaa): correction du design sur mobile fix(manage): affichage de la date du rendez-vous
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512CD788-CB8C-6D4A-9463-4CECC94F5849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D80144-1412-944D-BF05-7232A4947CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Date et heure</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Connexions au portail usager</t>
+  </si>
+  <si>
+    <t>Passages avec remise de courrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passages sans remise de courrier	</t>
   </si>
 </sst>
 </file>
@@ -252,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
@@ -296,6 +302,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -780,14 +789,24 @@
       </c>
       <c r="B29" s="9"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="9" t="s">
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="9"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="7" t="s">
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="7" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(stats): add 'actifs' in dashboard
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAA6AD4-5919-F646-B434-15BCAE1FF763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2942B137-03C2-8B48-8410-B7D08ECBFF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Date et heure</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>Mairies</t>
+  </si>
+  <si>
+    <t>Actifs (statut VALIDE)</t>
+  </si>
+  <si>
+    <t>Domiciliés actifs</t>
+  </si>
+  <si>
+    <t>Total des actifs</t>
   </si>
 </sst>
 </file>
@@ -261,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
@@ -309,6 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -632,7 +642,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B5" s="9"/>
       <c r="D5" s="9"/>
@@ -683,138 +693,162 @@
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="11" t="s">
-        <v>3</v>
+      <c r="A12" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="9" t="s">
-        <v>10</v>
+      <c r="A13" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="B13" s="9"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="9" t="s">
-        <v>11</v>
+      <c r="A14" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="9"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="9" t="s">
-        <v>12</v>
+      <c r="A15" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B15" s="9"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="B16" s="9"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="7" t="s">
-        <v>54</v>
+      <c r="A17" s="11" t="s">
+        <v>3</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="B18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B19" s="12"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="12" t="s">
-        <v>15</v>
+      <c r="A20" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="11" t="s">
-        <v>50</v>
+      <c r="A22" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="B23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B24" s="9"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="9" t="s">
-        <v>18</v>
+      <c r="A25" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="B26" s="9"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="9" t="s">
-        <v>20</v>
+      <c r="A27" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="B27" s="12"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="12" t="s">
-        <v>21</v>
+      <c r="A28" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="B28" s="9"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
+    </row>
+    <row r="36" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="16" t="s">
+    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
+    <row r="38" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A34" s="7" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="7" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(excel): delete useless column in excel
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2942B137-03C2-8B48-8410-B7D08ECBFF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558CA459-1E92-A743-AC06-B5F1E4D82113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats Globales" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Date et heure</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>Courriers remis</t>
-  </si>
-  <si>
-    <t>Pli non distribuable enregistré</t>
   </si>
   <si>
     <t>Avis de passage enregistrés</t>
@@ -217,7 +214,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy&quot; à &quot;hh:mm"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -246,8 +243,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -270,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
@@ -294,18 +304,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -315,10 +313,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,257 +610,252 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="7" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" style="7" customWidth="1"/>
-    <col min="5" max="1025" width="14.5" style="7" customWidth="1"/>
-    <col min="1026" max="16384" width="9.1640625" style="7"/>
+    <col min="1" max="1" width="26.6640625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="14" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" style="14" customWidth="1"/>
+    <col min="5" max="1025" width="14.5" style="14" customWidth="1"/>
+    <col min="1026" max="16384" width="9.1640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="11" t="s">
+      <c r="B1" s="13"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B16" s="9"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="11" t="s">
+      <c r="B15" s="12"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="12"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="9" t="s">
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="9" t="s">
+      <c r="B18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="12"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="9" t="s">
+      <c r="B19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="9" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="12"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="12" t="s">
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B26" s="9"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="12"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="9" t="s">
+      <c r="B25" s="12"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="12"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="16"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="9" t="s">
+      <c r="B28" s="12"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="9" t="s">
+      <c r="B29" s="12"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="9" t="s">
+      <c r="B30" s="12"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="9" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A35" s="9" t="s">
+    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
-        <v>24</v>
+      <c r="A36" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A39" s="7" t="s">
-        <v>51</v>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="14" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -889,58 +895,58 @@
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
@@ -2281,9 +2287,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2299,35 +2305,35 @@
     <col min="1023" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:1024" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="AMG1" s="15"/>
-      <c r="AMH1" s="15"/>
-      <c r="AMI1" s="15"/>
-      <c r="AMJ1" s="15"/>
+      <c r="AMG1" s="11"/>
+      <c r="AMH1" s="11"/>
+      <c r="AMI1" s="11"/>
+      <c r="AMJ1" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
fix(excel): update excel files
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558CA459-1E92-A743-AC06-B5F1E4D82113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2551FD-5D42-DE4B-8F25-7361FCC4A9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats Globales" sheetId="1" r:id="rId1"/>
@@ -868,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMN183"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
     </sheetView>
@@ -2287,7 +2287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>

</xml_diff>

<commit_message>
fix(structures): delete useless labels
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2551FD-5D42-DE4B-8F25-7361FCC4A9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DA9CA0-DC58-0241-B03D-A152AA432660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats Globales" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Date et heure</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Organisme agrée</t>
-  </si>
-  <si>
-    <t>CCAS</t>
   </si>
   <si>
     <t>CIAS</t>
@@ -195,9 +192,6 @@
     <t xml:space="preserve">Passages sans remise de courrier	</t>
   </si>
   <si>
-    <t>Mairies</t>
-  </si>
-  <si>
     <t>Actifs (statut VALIDE)</t>
   </si>
   <si>
@@ -205,6 +199,9 @@
   </si>
   <si>
     <t>Total des actifs</t>
+  </si>
+  <si>
+    <t>CCAS / Mairies / Communes</t>
   </si>
 </sst>
 </file>
@@ -610,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -645,7 +642,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="12"/>
       <c r="D4" s="12"/>
@@ -653,7 +650,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="12"/>
       <c r="D5" s="12"/>
@@ -705,14 +702,14 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="12"/>
       <c r="D13" s="16"/>
@@ -720,7 +717,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="12"/>
       <c r="D14" s="16"/>
@@ -728,7 +725,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="12"/>
       <c r="D15" s="16"/>
@@ -762,41 +759,41 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" s="12"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="12"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="B25" s="12"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="12"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="B25" s="12"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="12"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="B27" s="16"/>
     </row>
@@ -833,14 +830,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
+    <row r="34" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="16" x14ac:dyDescent="0.2">
@@ -848,14 +845,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="14" t="s">
-        <v>50</v>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -868,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMN183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
     </sheetView>
@@ -895,58 +887,58 @@
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
@@ -2307,28 +2299,28 @@
   <sheetData>
     <row r="1" spans="1:1024" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>45</v>
       </c>
       <c r="AMG1" s="11"/>
       <c r="AMH1" s="11"/>

</xml_diff>

<commit_message>
fix(admin): fix export in admin
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF517EA-1C42-9541-902E-6C8A2A3876E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871DE378-3724-094C-98B5-9F934738DFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Ville</t>
+  </si>
+  <si>
+    <t>Actifs</t>
   </si>
 </sst>
 </file>
@@ -472,11 +475,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AML183"/>
+  <dimension ref="A1:AMM183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" activeCellId="1" sqref="I1:I1048576 J1:J1048576"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -488,18 +491,18 @@
     <col min="5" max="5" width="11.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="5" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="3" customWidth="1"/>
-    <col min="9" max="11" width="13" style="5" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="33" style="3" customWidth="1"/>
-    <col min="14" max="14" width="7.83203125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="35" style="3" customWidth="1"/>
-    <col min="16" max="16" width="44.33203125" style="3" customWidth="1"/>
-    <col min="17" max="1026" width="8.6640625" style="3" customWidth="1"/>
-    <col min="1027" max="16384" width="9.1640625" style="7"/>
+    <col min="8" max="9" width="12.5" style="3" customWidth="1"/>
+    <col min="10" max="12" width="13" style="5" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="33" style="3" customWidth="1"/>
+    <col min="15" max="15" width="7.83203125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="35" style="3" customWidth="1"/>
+    <col min="17" max="17" width="44.33203125" style="3" customWidth="1"/>
+    <col min="18" max="1027" width="8.6640625" style="3" customWidth="1"/>
+    <col min="1028" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,1336 +528,1339 @@
         <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M2" s="4"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D3" s="4"/>
-      <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M3" s="4"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D4" s="4"/>
-      <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M4" s="4"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D5" s="4"/>
-      <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M5" s="4"/>
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D6" s="4"/>
-      <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M6" s="4"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D7" s="4"/>
-      <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M7" s="4"/>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D8" s="4"/>
-      <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M8" s="4"/>
+      <c r="N8" s="6"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D9" s="4"/>
-      <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M9" s="4"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D10" s="4"/>
-      <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M10" s="4"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D11" s="4"/>
-      <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M11" s="4"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D12" s="4"/>
-      <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M12" s="4"/>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D13" s="4"/>
-      <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M13" s="4"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D14" s="4"/>
-      <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M14" s="4"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D15" s="4"/>
-      <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="M15" s="4"/>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D17" s="4"/>
-      <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M17" s="4"/>
+      <c r="N17" s="6"/>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D18" s="4"/>
-      <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="6"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M18" s="4"/>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D19" s="4"/>
-      <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M19" s="4"/>
+      <c r="N19" s="6"/>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D20" s="4"/>
-      <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M20" s="4"/>
+      <c r="N20" s="6"/>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D21" s="4"/>
-      <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="6"/>
-    </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M21" s="4"/>
+      <c r="N21" s="6"/>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D22" s="4"/>
-      <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M22" s="4"/>
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D23" s="4"/>
-      <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="6"/>
-    </row>
-    <row r="24" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M23" s="4"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M24" s="4"/>
+      <c r="N24" s="6"/>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="26" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M26" s="4"/>
+      <c r="N26" s="6"/>
+    </row>
+    <row r="27" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D27" s="4"/>
-      <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="6"/>
-    </row>
-    <row r="28" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M27" s="4"/>
+      <c r="N27" s="6"/>
+    </row>
+    <row r="28" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D28" s="4"/>
-      <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="6"/>
-    </row>
-    <row r="29" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M28" s="4"/>
+      <c r="N28" s="6"/>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="6"/>
-    </row>
-    <row r="30" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M29" s="4"/>
+      <c r="N29" s="6"/>
+    </row>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D30" s="4"/>
-      <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="6"/>
-    </row>
-    <row r="31" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M30" s="4"/>
+      <c r="N30" s="6"/>
+    </row>
+    <row r="31" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D31" s="4"/>
-      <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="6"/>
-    </row>
-    <row r="32" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M31" s="4"/>
+      <c r="N31" s="6"/>
+    </row>
+    <row r="32" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D32" s="4"/>
-      <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="6"/>
-    </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M32" s="4"/>
+      <c r="N32" s="6"/>
+    </row>
+    <row r="33" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D33" s="4"/>
-      <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="6"/>
-    </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M33" s="4"/>
+      <c r="N33" s="6"/>
+    </row>
+    <row r="34" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D34" s="4"/>
-      <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="M34" s="6"/>
-    </row>
-    <row r="35" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M34" s="4"/>
+      <c r="N34" s="6"/>
+    </row>
+    <row r="35" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="36" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="37" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D37" s="4"/>
-      <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="6"/>
-    </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M37" s="4"/>
+      <c r="N37" s="6"/>
+    </row>
+    <row r="38" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="39" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D39" s="4"/>
-      <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="6"/>
-    </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M39" s="4"/>
+      <c r="N39" s="6"/>
+    </row>
+    <row r="40" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D40" s="4"/>
-      <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="6"/>
-    </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M40" s="4"/>
+      <c r="N40" s="6"/>
+    </row>
+    <row r="41" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D41" s="4"/>
-      <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="6"/>
-    </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M41" s="4"/>
+      <c r="N41" s="6"/>
+    </row>
+    <row r="42" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
-      <c r="M42" s="6"/>
-    </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M42" s="4"/>
+      <c r="N42" s="6"/>
+    </row>
+    <row r="43" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="6"/>
-    </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M43" s="4"/>
+      <c r="N43" s="6"/>
+    </row>
+    <row r="44" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="6"/>
-    </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M44" s="4"/>
+      <c r="N44" s="6"/>
+    </row>
+    <row r="45" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D45" s="4"/>
-      <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
-      <c r="M45" s="6"/>
-    </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M45" s="4"/>
+      <c r="N45" s="6"/>
+    </row>
+    <row r="46" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="47" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="48" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="49" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D49" s="4"/>
-      <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="6"/>
-    </row>
-    <row r="50" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M49" s="4"/>
+      <c r="N49" s="6"/>
+    </row>
+    <row r="50" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="51" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="52" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D52" s="4"/>
-      <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="6"/>
-    </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M52" s="4"/>
+      <c r="N52" s="6"/>
+    </row>
+    <row r="53" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D53" s="4"/>
       <c r="F53" s="4"/>
-      <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="6"/>
-    </row>
-    <row r="54" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M53" s="4"/>
+      <c r="N53" s="6"/>
+    </row>
+    <row r="54" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="55" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="56" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="57" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
-      <c r="M57" s="6"/>
-    </row>
-    <row r="58" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M57" s="4"/>
+      <c r="N57" s="6"/>
+    </row>
+    <row r="58" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
-      <c r="M58" s="6"/>
-    </row>
-    <row r="59" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M58" s="4"/>
+      <c r="N58" s="6"/>
+    </row>
+    <row r="59" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="60" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D60" s="4"/>
       <c r="F60" s="4"/>
-      <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
-      <c r="M60" s="6"/>
-    </row>
-    <row r="61" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M60" s="4"/>
+      <c r="N60" s="6"/>
+    </row>
+    <row r="61" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D61" s="4"/>
-      <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
-      <c r="M61" s="6"/>
-    </row>
-    <row r="62" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M61" s="4"/>
+      <c r="N61" s="6"/>
+    </row>
+    <row r="62" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D62" s="4"/>
-      <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
-      <c r="M62" s="6"/>
-    </row>
-    <row r="63" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M62" s="4"/>
+      <c r="N62" s="6"/>
+    </row>
+    <row r="63" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="64" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D64" s="4"/>
-      <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
-      <c r="M64" s="6"/>
-    </row>
-    <row r="65" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M64" s="4"/>
+      <c r="N64" s="6"/>
+    </row>
+    <row r="65" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="66" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D66" s="4"/>
       <c r="F66" s="4"/>
-      <c r="I66" s="4"/>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
-      <c r="M66" s="6"/>
-    </row>
-    <row r="67" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M66" s="4"/>
+      <c r="N66" s="6"/>
+    </row>
+    <row r="67" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D67" s="4"/>
-      <c r="I67" s="4"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
-      <c r="M67" s="6"/>
-    </row>
-    <row r="68" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M67" s="4"/>
+      <c r="N67" s="6"/>
+    </row>
+    <row r="68" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D68" s="4"/>
-      <c r="I68" s="4"/>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
-      <c r="M68" s="6"/>
-    </row>
-    <row r="69" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M68" s="4"/>
+      <c r="N68" s="6"/>
+    </row>
+    <row r="69" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D69" s="4"/>
-      <c r="I69" s="4"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="6"/>
-    </row>
-    <row r="70" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M69" s="4"/>
+      <c r="N69" s="6"/>
+    </row>
+    <row r="70" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D70" s="4"/>
-      <c r="I70" s="4"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
-      <c r="M70" s="6"/>
-    </row>
-    <row r="71" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M70" s="4"/>
+      <c r="N70" s="6"/>
+    </row>
+    <row r="71" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D71" s="4"/>
-      <c r="I71" s="4"/>
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
-      <c r="M71" s="6"/>
-    </row>
-    <row r="72" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M71" s="4"/>
+      <c r="N71" s="6"/>
+    </row>
+    <row r="72" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D72" s="4"/>
       <c r="F72" s="4"/>
-      <c r="I72" s="4"/>
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
-      <c r="M72" s="6"/>
-    </row>
-    <row r="73" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M72" s="4"/>
+      <c r="N72" s="6"/>
+    </row>
+    <row r="73" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="74" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D74" s="4"/>
-      <c r="I74" s="4"/>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
-      <c r="M74" s="6"/>
-    </row>
-    <row r="75" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M74" s="4"/>
+      <c r="N74" s="6"/>
+    </row>
+    <row r="75" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D75" s="4"/>
       <c r="F75" s="4"/>
-      <c r="I75" s="4"/>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
-      <c r="M75" s="6"/>
-    </row>
-    <row r="76" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M75" s="4"/>
+      <c r="N75" s="6"/>
+    </row>
+    <row r="76" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="77" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D77" s="4"/>
       <c r="F77" s="4"/>
-      <c r="I77" s="4"/>
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
-      <c r="M77" s="6"/>
-    </row>
-    <row r="78" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M77" s="4"/>
+      <c r="N77" s="6"/>
+    </row>
+    <row r="78" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="79" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D79" s="4"/>
-      <c r="I79" s="4"/>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
-      <c r="M79" s="6"/>
-    </row>
-    <row r="80" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M79" s="4"/>
+      <c r="N79" s="6"/>
+    </row>
+    <row r="80" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D80" s="4"/>
     </row>
-    <row r="81" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="81" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D81" s="4"/>
       <c r="F81" s="4"/>
-      <c r="I81" s="4"/>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
       <c r="L81" s="4"/>
-      <c r="M81" s="6"/>
-    </row>
-    <row r="82" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M81" s="4"/>
+      <c r="N81" s="6"/>
+    </row>
+    <row r="82" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D82" s="4"/>
-      <c r="I82" s="4"/>
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
-      <c r="M82" s="6"/>
-    </row>
-    <row r="83" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M82" s="4"/>
+      <c r="N82" s="6"/>
+    </row>
+    <row r="83" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="84" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D84" s="4"/>
-      <c r="I84" s="4"/>
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
-      <c r="M84" s="6"/>
-    </row>
-    <row r="85" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M84" s="4"/>
+      <c r="N84" s="6"/>
+    </row>
+    <row r="85" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D85" s="4"/>
       <c r="F85" s="4"/>
-      <c r="I85" s="4"/>
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
       <c r="L85" s="4"/>
-      <c r="M85" s="6"/>
-    </row>
-    <row r="86" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M85" s="4"/>
+      <c r="N85" s="6"/>
+    </row>
+    <row r="86" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D86" s="4"/>
-      <c r="I86" s="4"/>
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
-      <c r="M86" s="6"/>
-    </row>
-    <row r="87" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M86" s="4"/>
+      <c r="N86" s="6"/>
+    </row>
+    <row r="87" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="88" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D88" s="4"/>
       <c r="F88" s="4"/>
-      <c r="I88" s="4"/>
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
-      <c r="M88" s="6"/>
-    </row>
-    <row r="89" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M88" s="4"/>
+      <c r="N88" s="6"/>
+    </row>
+    <row r="89" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D89" s="4"/>
-      <c r="I89" s="4"/>
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
-      <c r="M89" s="6"/>
-    </row>
-    <row r="90" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M89" s="4"/>
+      <c r="N89" s="6"/>
+    </row>
+    <row r="90" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D90" s="4"/>
       <c r="F90" s="4"/>
-      <c r="I90" s="4"/>
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
-      <c r="M90" s="6"/>
-    </row>
-    <row r="91" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M90" s="4"/>
+      <c r="N90" s="6"/>
+    </row>
+    <row r="91" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D91" s="4"/>
       <c r="F91" s="4"/>
-      <c r="I91" s="4"/>
       <c r="J91" s="4"/>
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
-      <c r="M91" s="6"/>
-    </row>
-    <row r="92" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M91" s="4"/>
+      <c r="N91" s="6"/>
+    </row>
+    <row r="92" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D92" s="4"/>
       <c r="F92" s="4"/>
-      <c r="I92" s="4"/>
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
-      <c r="M92" s="6"/>
-    </row>
-    <row r="93" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M92" s="4"/>
+      <c r="N92" s="6"/>
+    </row>
+    <row r="93" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D93" s="4"/>
       <c r="F93" s="4"/>
-      <c r="I93" s="4"/>
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
-      <c r="M93" s="6"/>
-    </row>
-    <row r="94" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M93" s="4"/>
+      <c r="N93" s="6"/>
+    </row>
+    <row r="94" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D94" s="4"/>
-      <c r="I94" s="4"/>
       <c r="J94" s="4"/>
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
-      <c r="M94" s="6"/>
-    </row>
-    <row r="95" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M94" s="4"/>
+      <c r="N94" s="6"/>
+    </row>
+    <row r="95" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D95" s="4"/>
-      <c r="I95" s="4"/>
       <c r="J95" s="4"/>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
-      <c r="M95" s="6"/>
-    </row>
-    <row r="96" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M95" s="4"/>
+      <c r="N95" s="6"/>
+    </row>
+    <row r="96" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D96" s="4"/>
-      <c r="I96" s="4"/>
       <c r="J96" s="4"/>
       <c r="K96" s="4"/>
       <c r="L96" s="4"/>
-      <c r="M96" s="6"/>
-    </row>
-    <row r="97" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M96" s="4"/>
+      <c r="N96" s="6"/>
+    </row>
+    <row r="97" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D97" s="4"/>
       <c r="F97" s="4"/>
-      <c r="I97" s="4"/>
       <c r="J97" s="4"/>
       <c r="K97" s="4"/>
       <c r="L97" s="4"/>
-      <c r="M97" s="6"/>
-    </row>
-    <row r="98" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M97" s="4"/>
+      <c r="N97" s="6"/>
+    </row>
+    <row r="98" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D98" s="4"/>
-      <c r="I98" s="4"/>
       <c r="J98" s="4"/>
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
-      <c r="M98" s="6"/>
-    </row>
-    <row r="99" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M98" s="4"/>
+      <c r="N98" s="6"/>
+    </row>
+    <row r="99" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D99" s="4"/>
       <c r="F99" s="4"/>
-      <c r="I99" s="4"/>
       <c r="J99" s="4"/>
       <c r="K99" s="4"/>
       <c r="L99" s="4"/>
-      <c r="M99" s="6"/>
-    </row>
-    <row r="100" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M99" s="4"/>
+      <c r="N99" s="6"/>
+    </row>
+    <row r="100" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D100" s="4"/>
       <c r="F100" s="4"/>
-      <c r="I100" s="4"/>
       <c r="J100" s="4"/>
       <c r="K100" s="4"/>
       <c r="L100" s="4"/>
-      <c r="M100" s="6"/>
-    </row>
-    <row r="101" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M100" s="4"/>
+      <c r="N100" s="6"/>
+    </row>
+    <row r="101" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D101" s="4"/>
       <c r="F101" s="4"/>
-      <c r="I101" s="4"/>
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
       <c r="L101" s="4"/>
-      <c r="M101" s="6"/>
-    </row>
-    <row r="102" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M101" s="4"/>
+      <c r="N101" s="6"/>
+    </row>
+    <row r="102" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D102" s="4"/>
       <c r="F102" s="4"/>
-      <c r="I102" s="4"/>
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
       <c r="L102" s="4"/>
-      <c r="M102" s="6"/>
-    </row>
-    <row r="103" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M102" s="4"/>
+      <c r="N102" s="6"/>
+    </row>
+    <row r="103" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D103" s="4"/>
-      <c r="I103" s="4"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
       <c r="L103" s="4"/>
-      <c r="M103" s="6"/>
-    </row>
-    <row r="104" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M103" s="4"/>
+      <c r="N103" s="6"/>
+    </row>
+    <row r="104" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D104" s="4"/>
-      <c r="I104" s="4"/>
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
       <c r="L104" s="4"/>
-      <c r="M104" s="6"/>
-    </row>
-    <row r="105" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M104" s="4"/>
+      <c r="N104" s="6"/>
+    </row>
+    <row r="105" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D105" s="4"/>
       <c r="F105" s="4"/>
-      <c r="I105" s="4"/>
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
-      <c r="M105" s="6"/>
-    </row>
-    <row r="106" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M105" s="4"/>
+      <c r="N105" s="6"/>
+    </row>
+    <row r="106" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D106" s="4"/>
       <c r="F106" s="4"/>
-      <c r="I106" s="4"/>
       <c r="J106" s="4"/>
       <c r="K106" s="4"/>
       <c r="L106" s="4"/>
-      <c r="M106" s="6"/>
-    </row>
-    <row r="107" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M106" s="4"/>
+      <c r="N106" s="6"/>
+    </row>
+    <row r="107" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D107" s="4"/>
-      <c r="I107" s="4"/>
       <c r="J107" s="4"/>
       <c r="K107" s="4"/>
       <c r="L107" s="4"/>
-      <c r="M107" s="6"/>
-    </row>
-    <row r="108" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M107" s="4"/>
+      <c r="N107" s="6"/>
+    </row>
+    <row r="108" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D108" s="4"/>
       <c r="F108" s="4"/>
-      <c r="I108" s="4"/>
       <c r="J108" s="4"/>
       <c r="K108" s="4"/>
       <c r="L108" s="4"/>
-      <c r="M108" s="6"/>
-    </row>
-    <row r="109" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M108" s="4"/>
+      <c r="N108" s="6"/>
+    </row>
+    <row r="109" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D109" s="4"/>
       <c r="F109" s="4"/>
-      <c r="I109" s="4"/>
       <c r="J109" s="4"/>
       <c r="K109" s="4"/>
       <c r="L109" s="4"/>
-      <c r="M109" s="6"/>
-    </row>
-    <row r="110" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M109" s="4"/>
+      <c r="N109" s="6"/>
+    </row>
+    <row r="110" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D110" s="4"/>
-      <c r="I110" s="4"/>
       <c r="J110" s="4"/>
       <c r="K110" s="4"/>
       <c r="L110" s="4"/>
-      <c r="M110" s="6"/>
-    </row>
-    <row r="111" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M110" s="4"/>
+      <c r="N110" s="6"/>
+    </row>
+    <row r="111" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D111" s="4"/>
       <c r="F111" s="4"/>
-      <c r="I111" s="4"/>
       <c r="J111" s="4"/>
       <c r="K111" s="4"/>
       <c r="L111" s="4"/>
-      <c r="M111" s="6"/>
-    </row>
-    <row r="112" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M111" s="4"/>
+      <c r="N111" s="6"/>
+    </row>
+    <row r="112" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D112" s="4"/>
-      <c r="I112" s="4"/>
       <c r="J112" s="4"/>
       <c r="K112" s="4"/>
       <c r="L112" s="4"/>
-      <c r="M112" s="6"/>
-    </row>
-    <row r="113" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M112" s="4"/>
+      <c r="N112" s="6"/>
+    </row>
+    <row r="113" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D113" s="4"/>
-      <c r="I113" s="4"/>
       <c r="J113" s="4"/>
       <c r="K113" s="4"/>
       <c r="L113" s="4"/>
-      <c r="M113" s="6"/>
-    </row>
-    <row r="114" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M113" s="4"/>
+      <c r="N113" s="6"/>
+    </row>
+    <row r="114" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D114" s="4"/>
-      <c r="I114" s="4"/>
       <c r="J114" s="4"/>
       <c r="K114" s="4"/>
       <c r="L114" s="4"/>
-      <c r="M114" s="6"/>
-    </row>
-    <row r="115" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M114" s="4"/>
+      <c r="N114" s="6"/>
+    </row>
+    <row r="115" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D115" s="4"/>
       <c r="F115" s="4"/>
-      <c r="I115" s="4"/>
       <c r="J115" s="4"/>
       <c r="K115" s="4"/>
       <c r="L115" s="4"/>
-      <c r="M115" s="6"/>
-    </row>
-    <row r="116" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M115" s="4"/>
+      <c r="N115" s="6"/>
+    </row>
+    <row r="116" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D116" s="4"/>
       <c r="F116" s="4"/>
-      <c r="I116" s="4"/>
       <c r="J116" s="4"/>
       <c r="K116" s="4"/>
       <c r="L116" s="4"/>
-      <c r="M116" s="6"/>
-    </row>
-    <row r="117" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M116" s="4"/>
+      <c r="N116" s="6"/>
+    </row>
+    <row r="117" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D117" s="4"/>
       <c r="F117" s="4"/>
-      <c r="I117" s="4"/>
       <c r="J117" s="4"/>
       <c r="K117" s="4"/>
       <c r="L117" s="4"/>
-      <c r="M117" s="6"/>
-    </row>
-    <row r="118" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M117" s="4"/>
+      <c r="N117" s="6"/>
+    </row>
+    <row r="118" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D118" s="4"/>
       <c r="F118" s="4"/>
-      <c r="I118" s="4"/>
       <c r="J118" s="4"/>
       <c r="K118" s="4"/>
       <c r="L118" s="4"/>
-      <c r="M118" s="6"/>
-    </row>
-    <row r="119" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M118" s="4"/>
+      <c r="N118" s="6"/>
+    </row>
+    <row r="119" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D119" s="4"/>
       <c r="F119" s="4"/>
-      <c r="I119" s="4"/>
       <c r="J119" s="4"/>
       <c r="K119" s="4"/>
       <c r="L119" s="4"/>
-      <c r="M119" s="6"/>
-    </row>
-    <row r="120" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M119" s="4"/>
+      <c r="N119" s="6"/>
+    </row>
+    <row r="120" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D120" s="4"/>
       <c r="F120" s="4"/>
-      <c r="I120" s="4"/>
       <c r="J120" s="4"/>
       <c r="K120" s="4"/>
       <c r="L120" s="4"/>
-      <c r="M120" s="6"/>
-    </row>
-    <row r="121" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M120" s="4"/>
+      <c r="N120" s="6"/>
+    </row>
+    <row r="121" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D121" s="4"/>
-      <c r="I121" s="4"/>
       <c r="J121" s="4"/>
       <c r="K121" s="4"/>
       <c r="L121" s="4"/>
-      <c r="M121" s="6"/>
-    </row>
-    <row r="122" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M121" s="4"/>
+      <c r="N121" s="6"/>
+    </row>
+    <row r="122" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D122" s="4"/>
-      <c r="I122" s="4"/>
       <c r="J122" s="4"/>
       <c r="K122" s="4"/>
       <c r="L122" s="4"/>
-      <c r="M122" s="6"/>
-    </row>
-    <row r="123" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M122" s="4"/>
+      <c r="N122" s="6"/>
+    </row>
+    <row r="123" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D123" s="4"/>
-      <c r="I123" s="4"/>
       <c r="J123" s="4"/>
       <c r="K123" s="4"/>
       <c r="L123" s="4"/>
-      <c r="M123" s="6"/>
-    </row>
-    <row r="124" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M123" s="4"/>
+      <c r="N123" s="6"/>
+    </row>
+    <row r="124" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D124" s="4"/>
-      <c r="I124" s="4"/>
       <c r="J124" s="4"/>
       <c r="K124" s="4"/>
       <c r="L124" s="4"/>
-      <c r="M124" s="6"/>
-    </row>
-    <row r="125" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M124" s="4"/>
+      <c r="N124" s="6"/>
+    </row>
+    <row r="125" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D125" s="4"/>
-      <c r="I125" s="4"/>
       <c r="J125" s="4"/>
       <c r="K125" s="4"/>
       <c r="L125" s="4"/>
-      <c r="M125" s="6"/>
-    </row>
-    <row r="126" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M125" s="4"/>
+      <c r="N125" s="6"/>
+    </row>
+    <row r="126" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D126" s="4"/>
       <c r="F126" s="4"/>
-      <c r="I126" s="4"/>
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
       <c r="L126" s="4"/>
-      <c r="M126" s="6"/>
-    </row>
-    <row r="127" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M126" s="4"/>
+      <c r="N126" s="6"/>
+    </row>
+    <row r="127" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D127" s="4"/>
-      <c r="I127" s="4"/>
       <c r="J127" s="4"/>
       <c r="K127" s="4"/>
       <c r="L127" s="4"/>
-      <c r="M127" s="6"/>
-    </row>
-    <row r="128" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M127" s="4"/>
+      <c r="N127" s="6"/>
+    </row>
+    <row r="128" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D128" s="4"/>
-      <c r="I128" s="4"/>
       <c r="J128" s="4"/>
       <c r="K128" s="4"/>
       <c r="L128" s="4"/>
-      <c r="M128" s="6"/>
-    </row>
-    <row r="129" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M128" s="4"/>
+      <c r="N128" s="6"/>
+    </row>
+    <row r="129" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="130" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D130" s="4"/>
-      <c r="I130" s="4"/>
       <c r="J130" s="4"/>
       <c r="K130" s="4"/>
       <c r="L130" s="4"/>
-      <c r="M130" s="6"/>
-    </row>
-    <row r="131" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M130" s="4"/>
+      <c r="N130" s="6"/>
+    </row>
+    <row r="131" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="132" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D132" s="4"/>
       <c r="F132" s="4"/>
-      <c r="I132" s="4"/>
       <c r="J132" s="4"/>
       <c r="K132" s="4"/>
       <c r="L132" s="4"/>
-      <c r="M132" s="6"/>
-    </row>
-    <row r="133" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M132" s="4"/>
+      <c r="N132" s="6"/>
+    </row>
+    <row r="133" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D133" s="4"/>
-      <c r="I133" s="4"/>
       <c r="J133" s="4"/>
       <c r="K133" s="4"/>
       <c r="L133" s="4"/>
-      <c r="M133" s="6"/>
-    </row>
-    <row r="134" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M133" s="4"/>
+      <c r="N133" s="6"/>
+    </row>
+    <row r="134" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D134" s="4"/>
-      <c r="I134" s="4"/>
       <c r="J134" s="4"/>
       <c r="K134" s="4"/>
       <c r="L134" s="4"/>
-      <c r="M134" s="6"/>
-    </row>
-    <row r="135" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M134" s="4"/>
+      <c r="N134" s="6"/>
+    </row>
+    <row r="135" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D135" s="4"/>
-      <c r="I135" s="4"/>
       <c r="J135" s="4"/>
       <c r="K135" s="4"/>
       <c r="L135" s="4"/>
-      <c r="M135" s="6"/>
-    </row>
-    <row r="136" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M135" s="4"/>
+      <c r="N135" s="6"/>
+    </row>
+    <row r="136" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D136" s="4"/>
-      <c r="I136" s="4"/>
       <c r="J136" s="4"/>
       <c r="K136" s="4"/>
       <c r="L136" s="4"/>
-      <c r="M136" s="6"/>
-    </row>
-    <row r="137" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M136" s="4"/>
+      <c r="N136" s="6"/>
+    </row>
+    <row r="137" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="138" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="139" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D139" s="4"/>
-      <c r="I139" s="4"/>
       <c r="J139" s="4"/>
       <c r="K139" s="4"/>
       <c r="L139" s="4"/>
-      <c r="M139" s="6"/>
-    </row>
-    <row r="140" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M139" s="4"/>
+      <c r="N139" s="6"/>
+    </row>
+    <row r="140" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D140" s="4"/>
-      <c r="I140" s="4"/>
       <c r="J140" s="4"/>
       <c r="K140" s="4"/>
       <c r="L140" s="4"/>
-      <c r="M140" s="6"/>
-    </row>
-    <row r="141" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M140" s="4"/>
+      <c r="N140" s="6"/>
+    </row>
+    <row r="141" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D141" s="4"/>
-      <c r="I141" s="4"/>
       <c r="J141" s="4"/>
       <c r="K141" s="4"/>
       <c r="L141" s="4"/>
-      <c r="M141" s="6"/>
-    </row>
-    <row r="142" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M141" s="4"/>
+      <c r="N141" s="6"/>
+    </row>
+    <row r="142" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D142" s="4"/>
-      <c r="I142" s="4"/>
       <c r="J142" s="4"/>
       <c r="K142" s="4"/>
       <c r="L142" s="4"/>
-      <c r="M142" s="6"/>
-    </row>
-    <row r="143" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M142" s="4"/>
+      <c r="N142" s="6"/>
+    </row>
+    <row r="143" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D143" s="4"/>
-      <c r="I143" s="4"/>
       <c r="J143" s="4"/>
       <c r="K143" s="4"/>
       <c r="L143" s="4"/>
-      <c r="M143" s="6"/>
-    </row>
-    <row r="144" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M143" s="4"/>
+      <c r="N143" s="6"/>
+    </row>
+    <row r="144" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="145" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D145" s="4"/>
-      <c r="I145" s="4"/>
       <c r="J145" s="4"/>
       <c r="K145" s="4"/>
       <c r="L145" s="4"/>
-      <c r="M145" s="6"/>
-    </row>
-    <row r="146" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M145" s="4"/>
+      <c r="N145" s="6"/>
+    </row>
+    <row r="146" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D146" s="4"/>
-      <c r="I146" s="4"/>
       <c r="J146" s="4"/>
       <c r="K146" s="4"/>
       <c r="L146" s="4"/>
-      <c r="M146" s="6"/>
-    </row>
-    <row r="147" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M146" s="4"/>
+      <c r="N146" s="6"/>
+    </row>
+    <row r="147" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D147" s="4"/>
-      <c r="I147" s="4"/>
       <c r="J147" s="4"/>
       <c r="K147" s="4"/>
       <c r="L147" s="4"/>
-      <c r="M147" s="6"/>
-    </row>
-    <row r="148" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M147" s="4"/>
+      <c r="N147" s="6"/>
+    </row>
+    <row r="148" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D148" s="4"/>
     </row>
-    <row r="149" spans="4:13" x14ac:dyDescent="0.15">
+    <row r="149" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D149" s="4"/>
       <c r="F149" s="4"/>
-      <c r="I149" s="4"/>
       <c r="J149" s="4"/>
       <c r="K149" s="4"/>
       <c r="L149" s="4"/>
-      <c r="M149" s="6"/>
-    </row>
-    <row r="150" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M149" s="4"/>
+      <c r="N149" s="6"/>
+    </row>
+    <row r="150" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D150" s="4"/>
-      <c r="I150" s="4"/>
       <c r="J150" s="4"/>
       <c r="K150" s="4"/>
       <c r="L150" s="4"/>
-      <c r="M150" s="6"/>
-    </row>
-    <row r="151" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M150" s="4"/>
+      <c r="N150" s="6"/>
+    </row>
+    <row r="151" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D151" s="4"/>
-      <c r="I151" s="4"/>
       <c r="J151" s="4"/>
       <c r="K151" s="4"/>
       <c r="L151" s="4"/>
-      <c r="M151" s="6"/>
-    </row>
-    <row r="152" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M151" s="4"/>
+      <c r="N151" s="6"/>
+    </row>
+    <row r="152" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D152" s="4"/>
-      <c r="I152" s="4"/>
       <c r="J152" s="4"/>
       <c r="K152" s="4"/>
       <c r="L152" s="4"/>
-      <c r="M152" s="6"/>
-    </row>
-    <row r="153" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M152" s="4"/>
+      <c r="N152" s="6"/>
+    </row>
+    <row r="153" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D153" s="4"/>
-      <c r="I153" s="4"/>
       <c r="J153" s="4"/>
       <c r="K153" s="4"/>
       <c r="L153" s="4"/>
-      <c r="M153" s="6"/>
-    </row>
-    <row r="154" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M153" s="4"/>
+      <c r="N153" s="6"/>
+    </row>
+    <row r="154" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D154" s="4"/>
-      <c r="I154" s="4"/>
       <c r="J154" s="4"/>
       <c r="K154" s="4"/>
       <c r="L154" s="4"/>
-      <c r="M154" s="6"/>
-    </row>
-    <row r="155" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M154" s="4"/>
+      <c r="N154" s="6"/>
+    </row>
+    <row r="155" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D155" s="4"/>
-      <c r="I155" s="4"/>
       <c r="J155" s="4"/>
       <c r="K155" s="4"/>
       <c r="L155" s="4"/>
-      <c r="M155" s="6"/>
-    </row>
-    <row r="156" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M155" s="4"/>
+      <c r="N155" s="6"/>
+    </row>
+    <row r="156" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D156" s="4"/>
       <c r="F156" s="4"/>
-      <c r="I156" s="4"/>
       <c r="J156" s="4"/>
       <c r="K156" s="4"/>
       <c r="L156" s="4"/>
-      <c r="M156" s="6"/>
-    </row>
-    <row r="157" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M156" s="4"/>
+      <c r="N156" s="6"/>
+    </row>
+    <row r="157" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D157" s="4"/>
       <c r="F157" s="4"/>
-      <c r="I157" s="4"/>
       <c r="J157" s="4"/>
       <c r="K157" s="4"/>
       <c r="L157" s="4"/>
-      <c r="M157" s="6"/>
-    </row>
-    <row r="158" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M157" s="4"/>
+      <c r="N157" s="6"/>
+    </row>
+    <row r="158" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D158" s="4"/>
-      <c r="I158" s="4"/>
       <c r="J158" s="4"/>
       <c r="K158" s="4"/>
       <c r="L158" s="4"/>
-      <c r="M158" s="6"/>
-    </row>
-    <row r="159" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M158" s="4"/>
+      <c r="N158" s="6"/>
+    </row>
+    <row r="159" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D159" s="4"/>
-      <c r="I159" s="4"/>
       <c r="J159" s="4"/>
       <c r="K159" s="4"/>
       <c r="L159" s="4"/>
-      <c r="M159" s="6"/>
-    </row>
-    <row r="160" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M159" s="4"/>
+      <c r="N159" s="6"/>
+    </row>
+    <row r="160" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D160" s="4"/>
       <c r="F160" s="4"/>
-      <c r="I160" s="4"/>
       <c r="J160" s="4"/>
       <c r="K160" s="4"/>
       <c r="L160" s="4"/>
-      <c r="M160" s="6"/>
-    </row>
-    <row r="161" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M160" s="4"/>
+      <c r="N160" s="6"/>
+    </row>
+    <row r="161" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D161" s="4"/>
       <c r="F161" s="4"/>
-      <c r="I161" s="4"/>
       <c r="J161" s="4"/>
       <c r="K161" s="4"/>
       <c r="L161" s="4"/>
-      <c r="M161" s="6"/>
-    </row>
-    <row r="162" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M161" s="4"/>
+      <c r="N161" s="6"/>
+    </row>
+    <row r="162" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D162" s="4"/>
-      <c r="I162" s="4"/>
       <c r="J162" s="4"/>
       <c r="K162" s="4"/>
       <c r="L162" s="4"/>
-      <c r="M162" s="6"/>
-    </row>
-    <row r="163" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M162" s="4"/>
+      <c r="N162" s="6"/>
+    </row>
+    <row r="163" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D163" s="4"/>
-      <c r="I163" s="4"/>
       <c r="J163" s="4"/>
       <c r="K163" s="4"/>
       <c r="L163" s="4"/>
-      <c r="M163" s="6"/>
-    </row>
-    <row r="164" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M163" s="4"/>
+      <c r="N163" s="6"/>
+    </row>
+    <row r="164" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D164" s="4"/>
       <c r="F164" s="4"/>
-      <c r="I164" s="4"/>
       <c r="J164" s="4"/>
       <c r="K164" s="4"/>
       <c r="L164" s="4"/>
-      <c r="M164" s="6"/>
-    </row>
-    <row r="165" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M164" s="4"/>
+      <c r="N164" s="6"/>
+    </row>
+    <row r="165" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D165" s="4"/>
-      <c r="I165" s="4"/>
       <c r="J165" s="4"/>
       <c r="K165" s="4"/>
       <c r="L165" s="4"/>
-      <c r="M165" s="6"/>
-    </row>
-    <row r="166" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M165" s="4"/>
+      <c r="N165" s="6"/>
+    </row>
+    <row r="166" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D166" s="4"/>
-      <c r="I166" s="4"/>
       <c r="J166" s="4"/>
       <c r="K166" s="4"/>
       <c r="L166" s="4"/>
-      <c r="M166" s="6"/>
-    </row>
-    <row r="167" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M166" s="4"/>
+      <c r="N166" s="6"/>
+    </row>
+    <row r="167" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D167" s="4"/>
-      <c r="I167" s="4"/>
       <c r="J167" s="4"/>
       <c r="K167" s="4"/>
       <c r="L167" s="4"/>
-      <c r="M167" s="6"/>
-    </row>
-    <row r="168" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M167" s="4"/>
+      <c r="N167" s="6"/>
+    </row>
+    <row r="168" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D168" s="4"/>
-      <c r="I168" s="4"/>
       <c r="J168" s="4"/>
       <c r="K168" s="4"/>
       <c r="L168" s="4"/>
-      <c r="M168" s="6"/>
-    </row>
-    <row r="169" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M168" s="4"/>
+      <c r="N168" s="6"/>
+    </row>
+    <row r="169" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D169" s="4"/>
-      <c r="I169" s="4"/>
       <c r="J169" s="4"/>
       <c r="K169" s="4"/>
       <c r="L169" s="4"/>
-      <c r="M169" s="6"/>
-    </row>
-    <row r="170" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M169" s="4"/>
+      <c r="N169" s="6"/>
+    </row>
+    <row r="170" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D170" s="4"/>
-      <c r="I170" s="4"/>
       <c r="J170" s="4"/>
       <c r="K170" s="4"/>
       <c r="L170" s="4"/>
-      <c r="M170" s="6"/>
-    </row>
-    <row r="171" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M170" s="4"/>
+      <c r="N170" s="6"/>
+    </row>
+    <row r="171" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D171" s="4"/>
-      <c r="I171" s="4"/>
       <c r="J171" s="4"/>
       <c r="K171" s="4"/>
       <c r="L171" s="4"/>
-      <c r="M171" s="6"/>
-    </row>
-    <row r="172" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M171" s="4"/>
+      <c r="N171" s="6"/>
+    </row>
+    <row r="172" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D172" s="4"/>
-      <c r="I172" s="4"/>
       <c r="J172" s="4"/>
       <c r="K172" s="4"/>
       <c r="L172" s="4"/>
-      <c r="M172" s="6"/>
-    </row>
-    <row r="173" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M172" s="4"/>
+      <c r="N172" s="6"/>
+    </row>
+    <row r="173" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D173" s="4"/>
-      <c r="I173" s="4"/>
       <c r="J173" s="4"/>
       <c r="K173" s="4"/>
       <c r="L173" s="4"/>
-      <c r="M173" s="6"/>
-    </row>
-    <row r="174" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M173" s="4"/>
+      <c r="N173" s="6"/>
+    </row>
+    <row r="174" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D174" s="4"/>
-      <c r="I174" s="4"/>
       <c r="J174" s="4"/>
       <c r="K174" s="4"/>
       <c r="L174" s="4"/>
-      <c r="M174" s="6"/>
-    </row>
-    <row r="175" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M174" s="4"/>
+      <c r="N174" s="6"/>
+    </row>
+    <row r="175" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D175" s="4"/>
-      <c r="I175" s="4"/>
       <c r="J175" s="4"/>
       <c r="K175" s="4"/>
       <c r="L175" s="4"/>
-      <c r="M175" s="6"/>
-    </row>
-    <row r="176" spans="4:13" x14ac:dyDescent="0.15">
+      <c r="M175" s="4"/>
+      <c r="N175" s="6"/>
+    </row>
+    <row r="176" spans="4:14" x14ac:dyDescent="0.15">
       <c r="D176" s="4"/>
       <c r="F176" s="4"/>
-      <c r="I176" s="4"/>
       <c r="J176" s="4"/>
       <c r="K176" s="4"/>
       <c r="L176" s="4"/>
-      <c r="M176" s="6"/>
+      <c r="M176" s="4"/>
+      <c r="N176" s="6"/>
     </row>
     <row r="177" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D177" s="4"/>

</xml_diff>

<commit_message>
fix(frontend): fix transfer form
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
+++ b/packages/backend/src/excel/_templates/export-stats-deploiement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871DE378-3724-094C-98B5-9F934738DFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A33C15-10E4-E44F-8A3B-E0E29A287D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="760" windowWidth="29160" windowHeight="19380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
@@ -194,6 +194,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,8 +481,8 @@
   <dimension ref="A1:AMM183"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L164" sqref="L164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -490,8 +493,8 @@
     <col min="4" max="4" width="17.6640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="3" customWidth="1"/>
-    <col min="8" max="9" width="12.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="12" customWidth="1"/>
+    <col min="8" max="9" width="12.5" style="12" customWidth="1"/>
     <col min="10" max="12" width="13" style="5" customWidth="1"/>
     <col min="13" max="13" width="6.1640625" style="5" customWidth="1"/>
     <col min="14" max="14" width="33" style="3" customWidth="1"/>

</xml_diff>